<commit_message>
GĐ 1-2: Cấu trúc thư mục theo chức năng (user, project, task, comment).
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCE23B7-D72B-4423-97DE-EA0F8F6A3C1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8508CD66-4B79-46CA-9ED9-AFFFFA2EEA7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="141">
   <si>
     <t>STT</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>Ghi chú</t>
-  </si>
-  <si>
-    <t>Gợi ý cấu trúc thư mục Laravel (theo chức năng)</t>
   </si>
   <si>
     <t>- Tạo project Laravel
@@ -148,18 +145,332 @@
     <t>Libraries/Lệnh</t>
   </si>
   <si>
-    <t>laravel new task-manager-laravel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/7
-</t>
+    <t>5/7
+5/7</t>
+  </si>
+  <si>
+    <t>laravel new task-manager-laravel
+php artisan make:model Task -a</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── Http</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── Controllers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   ├── Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   │   └── CommentController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   ├── Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   │   └── ProjectController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   ├── Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   │   └── TaskController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   ├── User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   │   └── UserController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── Requests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       ├── Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       │   ├── StoreCommentRequest.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       │   └── UpdateCommentRequest.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       ├── Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       │   ├── StoreProjectRequest.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       │   └── UpdateProjectRequest.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       ├── Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       │   ├── StoreTaskRequest.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       │   └── UpdateTaskRequest.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       └── User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │           ├── StoreUserRequest.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │           └── UpdateUserRequest.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── Comment.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── User.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── Project.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── Task.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       └── User.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── Policies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── CommentPolicy.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── ProjectPolicy.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── TaskPolicy.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │       └── UserPolicy.php</t>
+  </si>
+  <si>
+    <t>Cấu trúc thư mục Laravel (theo chức năng)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+tạo 8 file (folder default chứa file mặc định của laravel)</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── factories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── UserFactory.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── CommentFactory.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── ProjectFactory.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── TaskFactory.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── UserFactory.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── migrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   ├── 0001_01_01_000000_create_users_table.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   ├── 0001_01_01_000001_create_cache_table.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── 0001_01_01_000002_create_jobs_table.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── 2025_07_05_021021_create_tasks_table.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── 2025_07_05_022217_create_users_table.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── 2025_07_05_022238_create_projects_table.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── 2025_07_05_022249_create_comments_table.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── seeders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── DatabaseSeeder.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── CommentSeeder.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── ProjectSeeder.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── TaskSeeder.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── UserSeeder.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    └── .gitignore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   ├── Controller.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   │   └── DashboardController.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── Providers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── AppServiceProvider.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    └── Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ├── Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        │   └── CommentService.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ├── Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        │   └── ProjectService.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ├── Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        │   └── TaskService.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        └── User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            └── UserService.php</t>
+  </si>
+  <si>
+    <t>views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── _form.blade.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── create.blade.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── edit.blade.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── index.blade.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── show.blade.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── index.blade.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── layouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── master.blade.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── partials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── _test.blade.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    └── welcome.blade.php</t>
+  </si>
+  <si>
+    <t>routes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── comment.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── dashboard.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── project.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   ├── task.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    │   └── user.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── console.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    └── web.php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +529,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -260,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -300,6 +618,8 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -312,22 +632,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,6 +744,50 @@
         <a:xfrm>
           <a:off x="4324350" y="781050"/>
           <a:ext cx="6081287" cy="5296359"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1630207</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>58004</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE865C10-DB21-4158-8A03-6527E3DF6DA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10620375" y="933450"/>
+          <a:ext cx="10259857" cy="6115904"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -722,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -737,36 +1101,36 @@
     <col min="8" max="8" width="32.7109375" style="8" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.28515625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.5703125" style="8" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="18"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -774,12 +1138,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -810,7 +1174,7 @@
         <v>28</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>29</v>
@@ -824,24 +1188,26 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="23" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -956,7 +1322,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -1004,82 +1370,670 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
   <dimension ref="B4:P166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="21"/>
-    <col min="2" max="2" width="9.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="9.140625" style="21"/>
-    <col min="15" max="15" width="33.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="78.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="9.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="9.140625" style="18"/>
+    <col min="15" max="15" width="33.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="78.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:16" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:15" s="29" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="16">
         <v>45843</v>
       </c>
-      <c r="O4" s="16"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="O12" s="22"/>
-    </row>
-    <row r="24" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-    </row>
-    <row r="25" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-    </row>
-    <row r="108" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="O4" s="30"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C12" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C17" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C18" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C19" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C20" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C23" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C26" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C27" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C28" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C29" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C30" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C31" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C32" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B108" s="24"/>
-      <c r="C108" s="24"/>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C109" s="22"/>
-      <c r="D109" s="22"/>
-      <c r="F109" s="22"/>
-      <c r="G109" s="25"/>
+      <c r="C108" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="116" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C116" s="22"/>
+      <c r="C116" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C118" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C119" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C120" s="18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C121" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C122" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C123" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C124" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C125" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C126" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C127" s="18" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="128" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C128" s="23"/>
-      <c r="D128" s="23"/>
+      <c r="C128" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D128" s="26"/>
     </row>
     <row r="129" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C129" s="23"/>
-      <c r="D129" s="23"/>
+      <c r="C129" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D129" s="26"/>
+    </row>
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C130" s="18" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="143" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B143" s="24"/>
-      <c r="E143" s="26"/>
-      <c r="F143" s="26"/>
-      <c r="G143" s="26"/>
-      <c r="H143" s="26"/>
-      <c r="I143" s="26"/>
-      <c r="J143" s="26"/>
-      <c r="K143" s="26"/>
-      <c r="L143" s="26"/>
+      <c r="E143" s="27"/>
+      <c r="F143" s="27"/>
+      <c r="G143" s="27"/>
+      <c r="H143" s="27"/>
+      <c r="I143" s="27"/>
+      <c r="J143" s="27"/>
+      <c r="K143" s="27"/>
+      <c r="L143" s="27"/>
     </row>
     <row r="144" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E144" s="27"/>
+      <c r="E144" s="28"/>
       <c r="F144" s="28"/>
       <c r="G144" s="28"/>
       <c r="H144" s="28"/>
@@ -1089,7 +2043,7 @@
       <c r="L144" s="28"/>
     </row>
     <row r="145" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E145" s="27"/>
+      <c r="E145" s="28"/>
       <c r="F145" s="28"/>
       <c r="G145" s="28"/>
       <c r="H145" s="28"/>
@@ -1139,7 +2093,7 @@
       <c r="L149" s="28"/>
     </row>
     <row r="150" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E150" s="27"/>
+      <c r="E150" s="28"/>
       <c r="F150" s="28"/>
       <c r="G150" s="28"/>
       <c r="H150" s="28"/>
@@ -1189,7 +2143,7 @@
       <c r="L154" s="28"/>
     </row>
     <row r="155" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E155" s="27"/>
+      <c r="E155" s="28"/>
       <c r="F155" s="28"/>
       <c r="G155" s="28"/>
       <c r="H155" s="28"/>
@@ -1239,7 +2193,7 @@
       <c r="L159" s="28"/>
     </row>
     <row r="160" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E160" s="27"/>
+      <c r="E160" s="28"/>
       <c r="F160" s="28"/>
       <c r="G160" s="28"/>
       <c r="H160" s="28"/>

</xml_diff>

<commit_message>
GĐ 1-7: Cài Laravel Breeze V2.3.7 để thiết lập hệ thống đăng ký, đăng nhập, và xác thực cơ bản cho ứng dụng Laravel.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266B8F02-CB50-480E-A754-D10B4FA4F85C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D977E63-1C37-44E2-B62E-5F41E386BA99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="165">
   <si>
     <t>STT</t>
   </si>
@@ -478,9 +478,6 @@
     <t>tạo 8 file (folder default chứa file mặc định của laravel)</t>
   </si>
   <si>
-    <t>9 file migrations (11 table, 3 table tạo từ file User)</t>
-  </si>
-  <si>
     <t>Bảng</t>
   </si>
   <si>
@@ -524,6 +521,16 @@
   </si>
   <si>
     <t>Phân loại Seeder / Factory cho từng bảng</t>
+  </si>
+  <si>
+    <t>7 file migrations (9 table, 3 table tạo từ file User)</t>
+  </si>
+  <si>
+    <t>php artisan make:seeder UserSeeder; php artisan db:seed --class=UserSeeder</t>
+  </si>
+  <si>
+    <t>Breeze laravel: composer require laravel/breeze --dev
+php artisan breeze:install (tạo frontend Blade mặc định)</t>
   </si>
 </sst>
 </file>
@@ -727,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -787,15 +794,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -813,6 +811,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -861,7 +860,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,7 +870,7 @@
   <dxfs count="2">
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </font>
       <fill>
         <patternFill>
@@ -879,7 +880,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </font>
       <fill>
         <patternFill>
@@ -1026,6 +1027,50 @@
         <a:xfrm>
           <a:off x="4857750" y="7181850"/>
           <a:ext cx="10440857" cy="5811061"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1087362</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>133867</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AD82A92-BC15-441A-9DCF-4BD2A2C2D4FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266825" y="25260300"/>
+          <a:ext cx="10831437" cy="3705742"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1322,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K20"/>
+  <dimension ref="A2:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1338,37 +1383,37 @@
     <col min="6" max="7" width="9.140625" style="8"/>
     <col min="8" max="8" width="32.7109375" style="8" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="70.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="49.5703125" style="8" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="38"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1376,12 +1421,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1419,19 +1464,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="41">
+      <c r="A7" s="39">
         <v>1</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="45" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="21"/>
@@ -1448,11 +1493,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="48"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="46"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -1469,62 +1514,70 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="48"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
         <v>139</v>
       </c>
       <c r="I9" s="25">
-        <v>45843</v>
+        <v>45844</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>145</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="48"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="I10" s="26"/>
-      <c r="J10" s="27"/>
+      <c r="I10" s="25">
+        <v>45845</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>163</v>
+      </c>
       <c r="K10" s="27"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="48"/>
+    <row r="11" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="I11" s="26"/>
-      <c r="J11" s="27"/>
+      <c r="I11" s="25">
+        <v>45845</v>
+      </c>
+      <c r="J11" s="51" t="s">
+        <v>164</v>
+      </c>
       <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="49"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -1534,18 +1587,18 @@
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
     </row>
-    <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>25</v>
@@ -1560,31 +1613,31 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="33"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="30"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -1592,65 +1645,65 @@
       <c r="E15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="33"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
     </row>
     <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="33"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="30"/>
     </row>
     <row r="17" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="33"/>
-    </row>
-    <row r="18" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="H17" s="28"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>25</v>
@@ -1660,29 +1713,8 @@
       <c r="J18" s="32"/>
       <c r="K18" s="33"/>
     </row>
-    <row r="19" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>7</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="34"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="36"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="9"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1697,11 +1729,11 @@
     <mergeCell ref="C7:C12"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>$G$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>$F$6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>$G$6</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1713,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
   <dimension ref="B4:P166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,8 +2097,8 @@
       <c r="C70" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D70" s="53" t="s">
-        <v>162</v>
+      <c r="D70" s="34" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
@@ -2074,13 +2106,13 @@
         <v>82</v>
       </c>
       <c r="D71" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E71" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="E71" s="13" t="s">
+      <c r="F71" s="13" t="s">
         <v>149</v>
-      </c>
-      <c r="F71" s="13" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.25">
@@ -2088,13 +2120,13 @@
         <v>83</v>
       </c>
       <c r="D72" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E72" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E72" s="13" t="s">
+      <c r="F72" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="F72" s="13" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
@@ -2102,13 +2134,13 @@
         <v>77</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E73" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F73" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="F73" s="13" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
@@ -2116,13 +2148,13 @@
         <v>84</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E74" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F74" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="F74" s="13" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
@@ -2130,13 +2162,13 @@
         <v>85</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E75" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F75" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="F75" s="13" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
@@ -2144,13 +2176,13 @@
         <v>86</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
@@ -2158,13 +2190,13 @@
         <v>87</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
@@ -2172,13 +2204,13 @@
         <v>88</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
@@ -2186,13 +2218,13 @@
         <v>89</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
@@ -2200,13 +2232,13 @@
         <v>90</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
@@ -2455,6 +2487,11 @@
     <row r="130" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C130" s="13" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="131" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B131" s="11">
+        <v>45845</v>
       </c>
     </row>
     <row r="143" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
GĐ 2-1: Xây dựng giao diện dashboard, tách logic controller sang service, thêm quan hệ Eloquent.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D977E63-1C37-44E2-B62E-5F41E386BA99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A39451-B110-4963-B346-8F3A2B40683B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="231">
   <si>
     <t>STT</t>
   </si>
@@ -531,13 +531,606 @@
   <si>
     <t>Breeze laravel: composer require laravel/breeze --dev
 php artisan breeze:install (tạo frontend Blade mặc định)</t>
+  </si>
+  <si>
+    <t>custom breeze: Giao diện (views/auth và views/layouts views/profile) -&gt;Route(routes-&gt;auth)-&gt;Controller(Controller/Auth/)-&gt;middleware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">composer require spatie/laravel-permission
+</t>
+  </si>
+  <si>
+    <t>Permission (spatie V 6.20)</t>
+  </si>
+  <si>
+    <t>super-admin</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>leader</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>✅</t>
+  </si>
+  <si>
+    <t>❌</t>
+  </si>
+  <si>
+    <t>dashboard.view</t>
+  </si>
+  <si>
+    <t>user.view</t>
+  </si>
+  <si>
+    <t>user.create</t>
+  </si>
+  <si>
+    <t>user.edit</t>
+  </si>
+  <si>
+    <t>user.soft-delete</t>
+  </si>
+  <si>
+    <t>user.restore</t>
+  </si>
+  <si>
+    <t>user.force-delete</t>
+  </si>
+  <si>
+    <t>user.assign</t>
+  </si>
+  <si>
+    <t>project.view</t>
+  </si>
+  <si>
+    <t>project.create</t>
+  </si>
+  <si>
+    <t>project.edit</t>
+  </si>
+  <si>
+    <t>project.soft-delete</t>
+  </si>
+  <si>
+    <t>project.restore</t>
+  </si>
+  <si>
+    <t>project.force-delete</t>
+  </si>
+  <si>
+    <t>project.assign</t>
+  </si>
+  <si>
+    <t>task.view</t>
+  </si>
+  <si>
+    <t>task.create</t>
+  </si>
+  <si>
+    <t>task.edit</t>
+  </si>
+  <si>
+    <t>task.soft-delete</t>
+  </si>
+  <si>
+    <t>task.restore</t>
+  </si>
+  <si>
+    <t>task.force-delete</t>
+  </si>
+  <si>
+    <t>task.assign</t>
+  </si>
+  <si>
+    <t>comment.view</t>
+  </si>
+  <si>
+    <t>comment.create</t>
+  </si>
+  <si>
+    <t>comment.edit</t>
+  </si>
+  <si>
+    <t>comment.soft-delete</t>
+  </si>
+  <si>
+    <t>comment.restore</t>
+  </si>
+  <si>
+    <t>comment.force-delete</t>
+  </si>
+  <si>
+    <t>✅own</t>
+  </si>
+  <si>
+    <t>gán role</t>
+  </si>
+  <si>
+    <t>Tình huống</t>
+  </si>
+  <si>
+    <t>Nên chọn</t>
+  </si>
+  <si>
+    <r>
+      <t>navbar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>footer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>sidebar</t>
+    </r>
+  </si>
+  <si>
+    <t>🟩 Partials (ít thay đổi, tĩnh)</t>
+  </si>
+  <si>
+    <r>
+      <t>alert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>badge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>form group</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>card</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nhỏ</t>
+    </r>
+  </si>
+  <si>
+    <t>🟦 Component (dùng lại nhiều + có nhiều biến thể)</t>
+  </si>
+  <si>
+    <r>
+      <t>table hiển thị</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>pagination</t>
+    </r>
+  </si>
+  <si>
+    <t>🔷 Component (tái sử dụng và truyền data dễ)</t>
+  </si>
+  <si>
+    <r>
+      <t>modal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>dropdown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>loading spinner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>toast</t>
+    </r>
+  </si>
+  <si>
+    <t>🔷 Component</t>
+  </si>
+  <si>
+    <t>Hiển thị 4 số liệu tổng quan: Tổng project, tổng task, tổng thành viên, tổng khách hàng.
+Mỗi ô có icon, màu nền, số lượng và nhãn rõ ràng.
+Mục đích: cho admin có cái nhìn nhanh về tình hình chung.</t>
+  </si>
+  <si>
+    <t>Hiển thị tỷ lệ dự án theo trạng thái.
+Giúp người xem thấy rõ phân bố các project: đang làm, hoàn thành, chờ xử lý, hủy.
+Loại doughnut trực quan, dễ hiểu.</t>
+  </si>
+  <si>
+    <t>Hiển thị các dự án có deadline gần nhất.
+Có thanh tiến độ (%) giúp đánh giá nhanh mức độ hoàn thành.
+Giúp ưu tiên xử lý đúng dự án.</t>
+  </si>
+  <si>
+    <t>Phân bố task theo trạng thái hiện tại.
+Tương tự doughnut project, nhưng cho task.</t>
+  </si>
+  <si>
+    <t>Biểu đồ cột thể hiện ai đang có nhiều task chưa hoàn thành nhất.
+Hỗ trợ đánh giá tải công việc, phân bổ lại khi cần.</t>
+  </si>
+  <si>
+    <t>Danh sách 4 task gần đây thay đổi trạng thái.
+Giúp theo dõi hoạt động mới nhất.</t>
+  </si>
+  <si>
+    <t>Hiển thị task quá hạn chưa hoàn thành.
+Rất quan trọng để quản lý rủi ro.</t>
+  </si>
+  <si>
+    <t>Hiển thị comment mới nhất liên quan task.
+Giúp theo dõi trao đổi, phản hồi.</t>
+  </si>
+  <si>
+    <t>Danh sách task của user đang đăng nhập.
+Có trạng thái và thời gian đến hạn hiển thị trực quan.</t>
+  </si>
+  <si>
+    <t>1. Laravel khuyến khích dùng Eloquent Relationships vì:</t>
+  </si>
+  <si>
+    <r>
+      <t>Dễ viết, dễ đọc:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Code ngắn gọn, rõ ràng, gần gũi với mô hình dữ liệu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tận dụng tính năng mạnh:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Eager loading (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), lazy loading, query builder cho quan hệ, các method hỗ trợ sẵn...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Giúp tránh lỗi N+1 query:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Khi dùng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>with()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Laravel sẽ load dữ liệu liên quan chỉ với vài câu query tối ưu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Dễ maintain &amp; refactor:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Khi cấu trúc DB thay đổi, chỉ sửa phần model quan hệ là xong, không phải sửa từng đoạn query thủ công.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hỗ trợ các thao tác CRUD thuận tiện:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Thêm/sửa/xóa quan hệ dễ dàng với các phương thức có sẵn như </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>save()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>attach()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>sync()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>...</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,8 +1203,35 @@
       <family val="1"/>
       <charset val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -621,6 +1241,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,7 +1360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -789,9 +1415,6 @@
     <xf numFmtId="16" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -812,6 +1435,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -860,8 +1525,14 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,7 +1583,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>80537</xdr:colOff>
+      <xdr:colOff>111017</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>187149</xdr:rowOff>
     </xdr:to>
@@ -956,9 +1627,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>1630207</xdr:colOff>
+      <xdr:colOff>530125</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>58004</xdr:rowOff>
+      <xdr:rowOff>73244</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1000,9 +1671,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>87182</xdr:colOff>
+      <xdr:colOff>110042</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>96061</xdr:rowOff>
+      <xdr:rowOff>111301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1044,9 +1715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1087362</xdr:colOff>
+      <xdr:colOff>1100697</xdr:colOff>
       <xdr:row>150</xdr:row>
-      <xdr:rowOff>133867</xdr:rowOff>
+      <xdr:rowOff>149107</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1071,6 +1742,50 @@
         <a:xfrm>
           <a:off x="1266825" y="25260300"/>
           <a:ext cx="10831437" cy="3705742"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1162050</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>644002</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>34709</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E5885FB-F3BE-4CCA-9119-8AE12605818A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12172950" y="25412700"/>
+          <a:ext cx="7220958" cy="3000794"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1369,11 +2084,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="8" bestFit="1" customWidth="1"/>
@@ -1384,36 +2099,36 @@
     <col min="8" max="8" width="32.7109375" style="8" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="70.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="49.5703125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="110.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="36"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -1421,12 +2136,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1464,19 +2179,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="39">
+      <c r="A7" s="52">
         <v>1</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="58" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="21"/>
@@ -1493,11 +2208,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="46"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="59"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -1514,11 +2229,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="46"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="59"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -1535,11 +2250,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="46"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="59"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -1548,17 +2263,17 @@
       <c r="I10" s="25">
         <v>45845</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="K10" s="27"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="46"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="59"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -1567,25 +2282,31 @@
       <c r="I11" s="25">
         <v>45845</v>
       </c>
-      <c r="J11" s="51" t="s">
+      <c r="J11" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="K11" s="27"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="47"/>
+      <c r="K11" s="35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="54"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="60"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="I12" s="26"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
+        <v>167</v>
+      </c>
+      <c r="I12" s="25">
+        <v>45851</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -1603,10 +2324,10 @@
       <c r="E13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="30"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1624,10 +2345,10 @@
       <c r="E14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1645,10 +2366,10 @@
       <c r="E15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
     </row>
     <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1666,10 +2387,10 @@
       <c r="E16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="30"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1687,10 +2408,10 @@
       <c r="E17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1708,10 +2429,10 @@
       <c r="E18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="33"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="32"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
@@ -1743,21 +2464,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
-  <dimension ref="B4:P166"/>
+  <dimension ref="B4:P214"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B202" sqref="B202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="9.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="13" customWidth="1"/>
     <col min="3" max="3" width="53.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="78.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="13" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="9.140625" style="13"/>
+    <col min="7" max="10" width="9.140625" style="13"/>
+    <col min="11" max="11" width="25.5703125" style="13" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="13"/>
     <col min="15" max="15" width="33.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="78.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="13"/>
@@ -2097,7 +2820,7 @@
       <c r="C70" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D70" s="34" t="s">
+      <c r="D70" s="33" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2515,7 +3238,7 @@
       <c r="K144" s="18"/>
       <c r="L144" s="18"/>
     </row>
-    <row r="145" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E145" s="18"/>
       <c r="F145" s="18"/>
       <c r="G145" s="18"/>
@@ -2525,7 +3248,7 @@
       <c r="K145" s="18"/>
       <c r="L145" s="18"/>
     </row>
-    <row r="146" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E146" s="18"/>
       <c r="F146" s="18"/>
       <c r="G146" s="18"/>
@@ -2535,7 +3258,7 @@
       <c r="K146" s="18"/>
       <c r="L146" s="18"/>
     </row>
-    <row r="147" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E147" s="18"/>
       <c r="F147" s="18"/>
       <c r="G147" s="18"/>
@@ -2545,7 +3268,7 @@
       <c r="K147" s="18"/>
       <c r="L147" s="18"/>
     </row>
-    <row r="148" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E148" s="18"/>
       <c r="F148" s="18"/>
       <c r="G148" s="18"/>
@@ -2555,7 +3278,7 @@
       <c r="K148" s="18"/>
       <c r="L148" s="18"/>
     </row>
-    <row r="149" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E149" s="18"/>
       <c r="F149" s="18"/>
       <c r="G149" s="18"/>
@@ -2565,7 +3288,7 @@
       <c r="K149" s="18"/>
       <c r="L149" s="18"/>
     </row>
-    <row r="150" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E150" s="18"/>
       <c r="F150" s="18"/>
       <c r="G150" s="18"/>
@@ -2575,7 +3298,7 @@
       <c r="K150" s="18"/>
       <c r="L150" s="18"/>
     </row>
-    <row r="151" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E151" s="18"/>
       <c r="F151" s="18"/>
       <c r="G151" s="18"/>
@@ -2585,7 +3308,7 @@
       <c r="K151" s="18"/>
       <c r="L151" s="18"/>
     </row>
-    <row r="152" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E152" s="18"/>
       <c r="F152" s="18"/>
       <c r="G152" s="18"/>
@@ -2595,7 +3318,7 @@
       <c r="K152" s="18"/>
       <c r="L152" s="18"/>
     </row>
-    <row r="153" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E153" s="18"/>
       <c r="F153" s="18"/>
       <c r="G153" s="18"/>
@@ -2605,9 +3328,14 @@
       <c r="K153" s="18"/>
       <c r="L153" s="18"/>
     </row>
-    <row r="154" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E154" s="18"/>
-      <c r="F154" s="18"/>
+    <row r="154" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B154" s="11">
+        <v>45851</v>
+      </c>
+      <c r="C154" s="36"/>
+      <c r="D154" s="36"/>
+      <c r="E154" s="36"/>
+      <c r="F154" s="36"/>
       <c r="G154" s="18"/>
       <c r="H154" s="18"/>
       <c r="I154" s="18"/>
@@ -2615,98 +3343,855 @@
       <c r="K154" s="18"/>
       <c r="L154" s="18"/>
     </row>
-    <row r="155" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E155" s="18"/>
-      <c r="F155" s="18"/>
-      <c r="G155" s="18"/>
-      <c r="H155" s="18"/>
-      <c r="I155" s="18"/>
-      <c r="J155" s="18"/>
-      <c r="K155" s="18"/>
+    <row r="155" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C155" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="D155" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="E155" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="F155" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="G155" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="H155" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="I155" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="J155" s="33"/>
+      <c r="K155">
+        <f>COUNTIF(D156:I183, D156) + COUNTIF(D156:I183, F159)</f>
+        <v>99</v>
+      </c>
       <c r="L155" s="18"/>
     </row>
-    <row r="156" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E156" s="18"/>
-      <c r="F156" s="18"/>
-      <c r="G156" s="18"/>
-      <c r="H156" s="18"/>
-      <c r="I156" s="18"/>
-      <c r="J156" s="18"/>
+    <row r="156" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C156" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="D156" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="E156" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F156" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G156" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="H156" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="I156" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="J156" s="40"/>
       <c r="K156" s="18"/>
       <c r="L156" s="18"/>
     </row>
-    <row r="157" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E157" s="18"/>
-      <c r="F157" s="18"/>
-      <c r="G157" s="18"/>
-      <c r="H157" s="18"/>
-      <c r="I157" s="18"/>
-      <c r="J157" s="18"/>
+    <row r="157" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C157" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="D157" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="E157" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F157" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G157" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="H157" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="I157" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="J157" s="40"/>
       <c r="K157" s="18"/>
       <c r="L157" s="18"/>
     </row>
-    <row r="158" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E158" s="18"/>
-      <c r="F158" s="18"/>
-      <c r="G158" s="18"/>
-      <c r="H158" s="18"/>
-      <c r="I158" s="18"/>
-      <c r="J158" s="18"/>
+    <row r="158" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C158" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="D158" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E158" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F158" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="G158" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H158" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I158" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J158" s="40"/>
       <c r="K158" s="18"/>
       <c r="L158" s="18"/>
     </row>
-    <row r="159" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E159" s="18"/>
-      <c r="F159" s="18"/>
-      <c r="G159" s="18"/>
-      <c r="H159" s="18"/>
-      <c r="I159" s="18"/>
-      <c r="J159" s="18"/>
+    <row r="159" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C159" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="D159" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E159" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F159" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="G159" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="H159" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="I159" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J159" s="40"/>
       <c r="K159" s="18"/>
       <c r="L159" s="18"/>
     </row>
-    <row r="160" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E160" s="18"/>
-      <c r="F160" s="18"/>
-      <c r="G160" s="18"/>
-      <c r="H160" s="18"/>
-      <c r="I160" s="18"/>
-      <c r="J160" s="18"/>
+    <row r="160" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C160" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="D160" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E160" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F160" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="G160" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H160" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I160" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J160" s="40"/>
       <c r="K160" s="18"/>
       <c r="L160" s="18"/>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E161" s="18"/>
-      <c r="F161" s="18"/>
-      <c r="G161" s="18"/>
-      <c r="H161" s="18"/>
-      <c r="I161" s="18"/>
-      <c r="J161" s="18"/>
+      <c r="C161" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="D161" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E161" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F161" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="G161" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H161" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I161" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J161" s="40"/>
       <c r="K161" s="18"/>
       <c r="L161" s="18"/>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E162" s="18"/>
-      <c r="F162" s="18"/>
-      <c r="G162" s="18"/>
-      <c r="H162" s="18"/>
-      <c r="I162" s="18"/>
-      <c r="J162" s="18"/>
+      <c r="C162" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="D162" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E162" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F162" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="G162" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="H162" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="I162" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="J162" s="40"/>
       <c r="K162" s="18"/>
       <c r="L162" s="18"/>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E163" s="18"/>
-      <c r="F163" s="18"/>
-      <c r="G163" s="18"/>
-      <c r="H163" s="18"/>
-      <c r="I163" s="18"/>
-      <c r="J163" s="18"/>
+      <c r="C163" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="D163" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E163" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F163" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="G163" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H163" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I163" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J163" s="46" t="s">
+        <v>205</v>
+      </c>
       <c r="K163" s="18"/>
       <c r="L163" s="18"/>
     </row>
+    <row r="164" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C164" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="D164" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="E164" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F164" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G164" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="H164" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="I164" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="J164" s="40"/>
+    </row>
+    <row r="165" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C165" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="D165" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E165" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F165" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G165" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H165" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I165" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J165" s="40"/>
+    </row>
     <row r="166" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B166" s="14"/>
+      <c r="C166" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D166" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E166" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F166" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G166" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H166" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I166" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J166" s="40"/>
+    </row>
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C167" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="D167" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E167" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F167" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="G167" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H167" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I167" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J167" s="40"/>
+    </row>
+    <row r="168" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C168" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="D168" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E168" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F168" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="G168" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H168" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I168" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J168" s="40"/>
+    </row>
+    <row r="169" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C169" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="D169" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E169" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F169" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="G169" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="H169" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="I169" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="J169" s="40"/>
+    </row>
+    <row r="170" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C170" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D170" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E170" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F170" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G170" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H170" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I170" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J170" s="40"/>
+    </row>
+    <row r="171" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C171" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="D171" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="E171" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F171" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G171" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="H171" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="I171" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="J171" s="40"/>
+    </row>
+    <row r="172" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C172" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="D172" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E172" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F172" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G172" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="H172" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I172" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J172" s="40"/>
+    </row>
+    <row r="173" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C173" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="D173" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E173" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F173" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G173" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="H173" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="I173" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J173" s="39"/>
+    </row>
+    <row r="174" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C174" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="D174" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E174" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F174" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G174" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H174" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I174" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J174" s="39"/>
+    </row>
+    <row r="175" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C175" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="D175" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E175" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F175" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G175" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H175" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I175" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J175" s="39"/>
+    </row>
+    <row r="176" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C176" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="D176" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E176" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F176" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="G176" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="H176" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="I176" s="45" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C177" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="D177" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E177" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F177" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G177" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="H177" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I177" s="41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C178" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="D178" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="E178" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F178" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G178" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="H178" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="I178" s="43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C179" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="D179" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E179" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F179" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="G179" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="H179" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="I179" s="41" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C180" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="D180" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E180" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F180" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="G180" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="H180" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="I180" s="41" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C181" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="D181" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E181" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F181" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="G181" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H181" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I181" s="41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C182" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="D182" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E182" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F182" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="G182" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="H182" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I182" s="41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C183" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="D183" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E183" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F183" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="G183" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="H183" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="I183" s="45" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="186" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B186" s="11"/>
+      <c r="C186" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="D186" s="38" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="187" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C187" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="D187" s="39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="188" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C188" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="D188" s="39" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="189" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C189" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="D189" s="39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="190" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C190" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="D190" s="39" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" ht="92.25" x14ac:dyDescent="0.4">
+      <c r="B193" s="11">
+        <v>45852</v>
+      </c>
+      <c r="C193" s="47" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C194" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="D194" s="47"/>
+    </row>
+    <row r="196" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C196" s="47" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C197" s="47" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C198" s="47" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C199" s="47" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C200" s="47" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C201" s="47" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C202" s="47" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B204" s="11">
+        <v>45853</v>
+      </c>
+      <c r="C204" s="64" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C205" s="65"/>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C206" s="66" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C207" s="65"/>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C208" s="66" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C209" s="65"/>
+    </row>
+    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C210" s="66" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C211" s="65"/>
+    </row>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C212" s="66" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C213" s="65"/>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C214" s="66" t="s">
+        <v>230</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GĐ 1-4-4: Cập nhật lại cấu trúc bảng projects và tasks (thêm slug, sửa unique). Điều chỉnh factory & seeder. Seed lại toàn bộ dữ liệu.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A39451-B110-4963-B346-8F3A2B40683B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADE1BA0-3CBF-4377-B32F-D9A855532368}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="253">
   <si>
     <t>STT</t>
   </si>
@@ -1125,12 +1125,162 @@
       <t>...</t>
     </r>
   </si>
+  <si>
+    <t>Tạo giao diện</t>
+  </si>
+  <si>
+    <t>Hiển thị số liệu</t>
+  </si>
+  <si>
+    <t>composer require jeroennoten/laravel-adminlte 
+php artisan adminlte:install</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Admin tạo tài khoản</t>
+  </si>
+  <si>
+    <t>Gửi mail xác minh</t>
+  </si>
+  <si>
+    <t>Cần đăng nhập thủ công</t>
+  </si>
+  <si>
+    <t>✅ (email + password)</t>
+  </si>
+  <si>
+    <t>Click link xác minh email</t>
+  </si>
+  <si>
+    <t>✅ → login thủ công</t>
+  </si>
+  <si>
+    <t>✅ → login tự động luôn</t>
+  </si>
+  <si>
+    <t>Xác minh tài khoản</t>
+  </si>
+  <si>
+    <t>Middleware</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">✅ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>signed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bắt buộc URL phải là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Signed URL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (có chữ ký bảo mật)</t>
+    </r>
+  </si>
+  <si>
+    <t>Laravel tự tạo link ký bằng secret key → không ai có thể "đoán" link xác minh</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ngăn chặn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>giả mạo URL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hoặc chỉnh sửa thủ công</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">✅ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>throttle:6,1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Giới hạn request: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tối đa 6 lần mỗi 1 phút</t>
+    </r>
+  </si>
+  <si>
+    <t>Tránh bị spam xác minh email</t>
+  </si>
+  <si>
+    <t>Nếu vượt quá thì sẽ bị chặn (HTTP 429 – Too Many Requests)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1229,6 +1379,29 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1360,7 +1533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1477,6 +1650,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1526,13 +1726,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2082,10 +2282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K19"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2104,31 +2304,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="49"/>
+      <c r="E3" s="58"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="49"/>
+      <c r="E4" s="58"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2136,12 +2336,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="50" t="s">
+      <c r="H5" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2179,19 +2379,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="52">
+      <c r="A7" s="61">
         <v>1</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="67" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="21"/>
@@ -2208,11 +2408,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="59"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="68"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2229,11 +2429,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="59"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -2250,11 +2450,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="59"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -2269,11 +2469,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="59"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="68"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -2290,11 +2490,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="60"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="69"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -2308,57 +2508,59 @@
       </c>
       <c r="K12" s="26"/>
     </row>
-    <row r="13" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+    <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="51">
         <v>2</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="29"/>
-    </row>
-    <row r="14" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="I13" s="25">
+        <v>45854</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="K13" s="26"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="56"/>
+      <c r="H14" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="I14" s="25">
+        <v>45856</v>
+      </c>
       <c r="J14" s="28"/>
       <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -2367,78 +2569,99 @@
         <v>25</v>
       </c>
       <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
+      <c r="I15" s="25"/>
       <c r="J15" s="28"/>
       <c r="K15" s="29"/>
     </row>
     <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
+      <c r="I16" s="25"/>
       <c r="J16" s="28"/>
       <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="27"/>
-      <c r="I17" s="28"/>
+      <c r="I17" s="25"/>
       <c r="J17" s="28"/>
       <c r="K17" s="29"/>
     </row>
-    <row r="18" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="32"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="9"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="29"/>
+    </row>
+    <row r="19" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>7</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="32"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="14">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -2448,8 +2671,13 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E15:E1048576 E1:E13">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$G$6</formula>
     </cfRule>
@@ -2464,10 +2692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
-  <dimension ref="B4:P214"/>
+  <dimension ref="B4:P233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B202" sqref="B202"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K167" sqref="K167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4149,48 +4377,165 @@
       <c r="B204" s="11">
         <v>45853</v>
       </c>
-      <c r="C204" s="64" t="s">
+      <c r="C204" s="48" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C205" s="65"/>
+      <c r="C205" s="49"/>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C206" s="66" t="s">
+      <c r="C206" s="50" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C207" s="65"/>
+      <c r="C207" s="49"/>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C208" s="66" t="s">
+      <c r="C208" s="50" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C209" s="65"/>
-    </row>
-    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C210" s="66" t="s">
+    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C209" s="49"/>
+    </row>
+    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C210" s="50" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C211" s="65"/>
-    </row>
-    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C212" s="66" t="s">
+    <row r="211" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C211" s="49"/>
+    </row>
+    <row r="212" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C212" s="50" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C213" s="65"/>
-    </row>
-    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C214" s="66" t="s">
+    <row r="213" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C213" s="49"/>
+    </row>
+    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C214" s="50" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="217" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B217" s="11">
+        <v>45857</v>
+      </c>
+      <c r="C217" s="73" t="s">
+        <v>243</v>
+      </c>
+      <c r="D217" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="E217" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="G217" s="74" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C218" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="D218" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="E218" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="G218"/>
+    </row>
+    <row r="219" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C219" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="D219" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="E219" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="G219" s="75" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C220" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="D220" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="E220" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="G220" s="49"/>
+    </row>
+    <row r="221" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C221" s="39" t="s">
+        <v>240</v>
+      </c>
+      <c r="D221" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="E221" s="39" t="s">
+        <v>242</v>
+      </c>
+      <c r="G221" s="49" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="222" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G222" s="49"/>
+    </row>
+    <row r="223" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G223" s="49" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="224" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G224" s="49"/>
+    </row>
+    <row r="225" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G225" s="49" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="226" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G226"/>
+    </row>
+    <row r="227" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G227" s="75" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="228" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G228" s="49"/>
+    </row>
+    <row r="229" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G229" s="49" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="230" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G230" s="49"/>
+    </row>
+    <row r="231" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G231" s="49" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="232" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G232" s="49"/>
+    </row>
+    <row r="233" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G233" s="49" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GĐ 2-1-1: Cập nhật giao diện dashboard và các view, service, controller liên quan.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADE1BA0-3CBF-4377-B32F-D9A855532368}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E0FC3D-D6B5-405A-A5CA-3F2184EBAB04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="264">
   <si>
     <t>STT</t>
   </si>
@@ -529,13 +529,6 @@
     <t>php artisan make:seeder UserSeeder; php artisan db:seed --class=UserSeeder</t>
   </si>
   <si>
-    <t>Breeze laravel: composer require laravel/breeze --dev
-php artisan breeze:install (tạo frontend Blade mặc định)</t>
-  </si>
-  <si>
-    <t>custom breeze: Giao diện (views/auth và views/layouts views/profile) -&gt;Route(routes-&gt;auth)-&gt;Controller(Controller/Auth/)-&gt;middleware</t>
-  </si>
-  <si>
     <t xml:space="preserve">composer require spatie/laravel-permission
 </t>
   </si>
@@ -1274,13 +1267,99 @@
   </si>
   <si>
     <t>Nếu vượt quá thì sẽ bị chặn (HTTP 429 – Too Many Requests)</t>
+  </si>
+  <si>
+    <t>composer require --dev barryvdh/laravel-ide-helper</t>
+  </si>
+  <si>
+    <t>Laravel IDE Helper</t>
+  </si>
+  <si>
+    <t>custom breeze: Giao diện (views/auth và views/layouts views/profile) -&gt;Route(routes-&gt;auth)-&gt;Controller(Controller/Auth/)-&gt;middleware
+Laravel IDE Helper: hỗ trợ intelephense đọc code</t>
+  </si>
+  <si>
+    <t>php artisan ide-helper:generate</t>
+  </si>
+  <si>
+    <t>Breeze laravel: composer require laravel/breeze --dev
+php artisan breeze:install (tạo frontend Blade mặc định)
+composer require --dev barryvdh/laravel-ide-helper -&gt; php artisan ide-helper:generate</t>
+  </si>
+  <si>
+    <t>Ưu điểm của Policy</t>
+  </si>
+  <si>
+    <t>Giúp code tách bạch: logic phân quyền không nằm rải rác trong controller mà tập trung trong Policy.</t>
+  </si>
+  <si>
+    <t>Dễ test, dễ mở rộng khi có nhiều rules phức tạp.</t>
+  </si>
+  <si>
+    <t>Là một phần của Laravel Authorization system rất mạnh mẽ.</t>
+  </si>
+  <si>
+    <t>1. Policy là gì?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Policy là một class dùng để </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>quy định quyền truy cập (authorization)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cho các hành động (action) trên một </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>model cụ thể</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (ví dụ: Project, Post, User,...).</t>
+    </r>
+  </si>
+  <si>
+    <t>Nó giúp tách biệt logic phân quyền ra khỏi controller, giúp code sạch, dễ bảo trì.</t>
+  </si>
+  <si>
+    <t>Policy kiểm soát “ai được làm gì trên đối tượng nào” (ví dụ: ai được xem, sửa, xóa một Project).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1402,6 +1481,14 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1533,7 +1620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1611,9 +1698,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1659,6 +1743,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1724,15 +1821,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1986,6 +2074,50 @@
         <a:xfrm>
           <a:off x="12172950" y="25412700"/>
           <a:ext cx="7220958" cy="3000794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>134471</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1430</xdr:colOff>
+      <xdr:row>242</xdr:row>
+      <xdr:rowOff>183203</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6880AC49-351D-4A87-B3EC-097F665259DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1826559" y="49989441"/>
+          <a:ext cx="8649907" cy="3115110"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2285,7 +2417,7 @@
   <dimension ref="A2:K20"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2304,31 +2436,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="58"/>
+      <c r="E3" s="62"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="58"/>
+      <c r="E4" s="62"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2336,12 +2468,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2379,19 +2511,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="61">
+      <c r="A7" s="65">
         <v>1</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="71" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="21"/>
@@ -2408,11 +2540,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="68"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="72"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2429,11 +2561,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="68"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="72"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -2450,11 +2582,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="68"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="72"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -2468,12 +2600,12 @@
       </c>
       <c r="K10" s="26"/>
     </row>
-    <row r="11" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="68"/>
+    <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="66"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="72"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -2483,68 +2615,68 @@
         <v>45845</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="K11" s="35" t="s">
-        <v>165</v>
+        <v>255</v>
+      </c>
+      <c r="K11" s="54" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="69"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I12" s="25">
         <v>45851</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="51">
+      <c r="A13" s="55">
         <v>2</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="55" t="s">
+      <c r="E13" s="59" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="27" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I13" s="25">
         <v>45854</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="56"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="60"/>
       <c r="H14" s="27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I14" s="25">
         <v>45856</v>
@@ -2692,10 +2824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
-  <dimension ref="B4:P233"/>
+  <dimension ref="B4:P250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K167" sqref="K167"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3560,10 +3692,10 @@
       <c r="B154" s="11">
         <v>45851</v>
       </c>
-      <c r="C154" s="36"/>
-      <c r="D154" s="36"/>
-      <c r="E154" s="36"/>
-      <c r="F154" s="36"/>
+      <c r="C154" s="35"/>
+      <c r="D154" s="35"/>
+      <c r="E154" s="35"/>
+      <c r="F154" s="35"/>
       <c r="G154" s="18"/>
       <c r="H154" s="18"/>
       <c r="I154" s="18"/>
@@ -3572,970 +3704,1023 @@
       <c r="L154" s="18"/>
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C155" s="38" t="s">
+      <c r="C155" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="D155" s="38" t="s">
+      <c r="D155" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="E155" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F155" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="E155" s="38" t="s">
+      <c r="G155" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="F155" s="38" t="s">
+      <c r="H155" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="G155" s="38" t="s">
+      <c r="I155" s="37" t="s">
         <v>171</v>
-      </c>
-      <c r="H155" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="I155" s="38" t="s">
-        <v>173</v>
       </c>
       <c r="J155" s="33"/>
       <c r="K155">
         <f>COUNTIF(D156:I183, D156) + COUNTIF(D156:I183, F159)</f>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L155" s="18"/>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C156" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="D156" s="43" t="s">
+      <c r="C156" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="E156" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="F156" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="G156" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="H156" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="I156" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="J156" s="40"/>
+      <c r="D156" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E156" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="F156" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="G156" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H156" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="I156" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="J156" s="39"/>
       <c r="K156" s="18"/>
       <c r="L156" s="18"/>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C157" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="D157" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="E157" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="F157" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="G157" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="H157" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="I157" s="43" t="s">
+      <c r="C157" s="41" t="s">
         <v>175</v>
       </c>
-      <c r="J157" s="40"/>
+      <c r="D157" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E157" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="F157" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="G157" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H157" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="I157" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="J157" s="39"/>
       <c r="K157" s="18"/>
       <c r="L157" s="18"/>
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C158" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="D158" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E158" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F158" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="G158" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H158" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I158" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J158" s="40"/>
+      <c r="C158" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="D158" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E158" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F158" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G158" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H158" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I158" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J158" s="39"/>
       <c r="K158" s="18"/>
       <c r="L158" s="18"/>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C159" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="D159" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E159" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F159" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="G159" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="H159" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="I159" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J159" s="40"/>
+      <c r="C159" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="D159" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E159" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F159" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="G159" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="H159" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="I159" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="J159" s="39"/>
       <c r="K159" s="18"/>
       <c r="L159" s="18"/>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C160" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="D160" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E160" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F160" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="G160" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H160" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I160" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J160" s="40"/>
+      <c r="C160" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="D160" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E160" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F160" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G160" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H160" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I160" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J160" s="39"/>
       <c r="K160" s="18"/>
       <c r="L160" s="18"/>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C161" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="D161" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E161" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F161" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="G161" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H161" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I161" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J161" s="40"/>
+      <c r="C161" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="D161" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E161" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F161" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G161" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H161" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I161" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J161" s="39"/>
       <c r="K161" s="18"/>
       <c r="L161" s="18"/>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C162" s="44" t="s">
-        <v>182</v>
-      </c>
-      <c r="D162" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="E162" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="F162" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="G162" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="H162" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="I162" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="J162" s="40"/>
+      <c r="C162" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="D162" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E162" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F162" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="G162" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="H162" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="I162" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="J162" s="39"/>
       <c r="K162" s="18"/>
       <c r="L162" s="18"/>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C163" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="D163" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E163" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F163" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="G163" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H163" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I163" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J163" s="46" t="s">
-        <v>205</v>
+      <c r="C163" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="D163" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E163" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F163" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G163" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H163" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I163" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J163" s="45" t="s">
+        <v>203</v>
       </c>
       <c r="K163" s="18"/>
       <c r="L163" s="18"/>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C164" s="42" t="s">
-        <v>184</v>
-      </c>
-      <c r="D164" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="E164" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="F164" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="G164" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="H164" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="I164" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="J164" s="40"/>
+      <c r="C164" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D164" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E164" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="F164" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="G164" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H164" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="I164" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="J164" s="39"/>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C165" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="D165" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E165" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F165" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G165" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H165" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I165" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J165" s="40"/>
+      <c r="C165" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="D165" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E165" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F165" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G165" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H165" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I165" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J165" s="39"/>
     </row>
     <row r="166" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B166" s="14"/>
-      <c r="C166" s="37" t="s">
+      <c r="C166" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="D166" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E166" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F166" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G166" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H166" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I166" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J166" s="39"/>
+    </row>
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C167" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="D167" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E167" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F167" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G167" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H167" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I167" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J167" s="39"/>
+    </row>
+    <row r="168" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C168" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D166" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E166" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F166" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G166" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H166" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I166" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J166" s="40"/>
-    </row>
-    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C167" s="37" t="s">
+      <c r="D168" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E168" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F168" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G168" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H168" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I168" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J168" s="39"/>
+    </row>
+    <row r="169" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C169" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="D167" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E167" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F167" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="G167" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H167" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I167" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J167" s="40"/>
-    </row>
-    <row r="168" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C168" s="37" t="s">
+      <c r="D169" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E169" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F169" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="G169" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="H169" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="I169" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="J169" s="39"/>
+    </row>
+    <row r="170" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C170" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="D168" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E168" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F168" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="G168" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H168" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I168" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J168" s="40"/>
-    </row>
-    <row r="169" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C169" s="44" t="s">
+      <c r="D170" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E170" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F170" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G170" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H170" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I170" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J170" s="39"/>
+    </row>
+    <row r="171" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C171" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="D169" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="E169" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="F169" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="G169" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="H169" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="I169" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="J169" s="40"/>
-    </row>
-    <row r="170" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C170" s="37" t="s">
+      <c r="D171" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E171" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="F171" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="G171" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H171" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="I171" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="J171" s="39"/>
+    </row>
+    <row r="172" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C172" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="D170" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E170" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F170" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G170" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H170" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I170" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J170" s="40"/>
-    </row>
-    <row r="171" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C171" s="42" t="s">
+      <c r="D172" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E172" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F172" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G172" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="H172" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I172" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J172" s="39"/>
+    </row>
+    <row r="173" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C173" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="D171" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="E171" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="F171" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="G171" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="H171" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="I171" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="J171" s="40"/>
-    </row>
-    <row r="172" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C172" s="37" t="s">
+      <c r="D173" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E173" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F173" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G173" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="H173" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="I173" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J173" s="38"/>
+    </row>
+    <row r="174" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C174" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="D172" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E172" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F172" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G172" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="H172" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I172" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J172" s="40"/>
-    </row>
-    <row r="173" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C173" s="37" t="s">
+      <c r="D174" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E174" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F174" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G174" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H174" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I174" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J174" s="38"/>
+    </row>
+    <row r="175" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C175" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="D173" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E173" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F173" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G173" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="H173" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="I173" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J173" s="39"/>
-    </row>
-    <row r="174" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C174" s="37" t="s">
+      <c r="D175" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E175" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F175" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G175" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H175" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I175" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J175" s="38"/>
+    </row>
+    <row r="176" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C176" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="D174" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E174" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F174" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G174" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H174" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I174" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J174" s="39"/>
-    </row>
-    <row r="175" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C175" s="37" t="s">
+      <c r="D176" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E176" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F176" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="G176" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="H176" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="I176" s="44" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C177" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="D175" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E175" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F175" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G175" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H175" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I175" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="J175" s="39"/>
-    </row>
-    <row r="176" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C176" s="44" t="s">
+      <c r="D177" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E177" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F177" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G177" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="H177" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I177" s="40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C178" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="D176" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="E176" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="F176" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="G176" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="H176" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="I176" s="45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C177" s="37" t="s">
+      <c r="D178" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E178" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="F178" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="G178" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H178" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="I178" s="42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C179" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="D177" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E177" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F177" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G177" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="H177" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I177" s="41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C178" s="42" t="s">
+      <c r="D179" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E179" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F179" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G179" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="H179" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="I179" s="40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C180" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="D178" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="E178" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="F178" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="G178" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="H178" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="I178" s="43" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C179" s="37" t="s">
+      <c r="D180" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E180" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F180" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="G180" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="H180" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="I180" s="40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C181" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="D179" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E179" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F179" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="G179" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="H179" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="I179" s="41" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C180" s="37" t="s">
+      <c r="D181" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E181" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F181" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G181" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H181" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I181" s="40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C182" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="D180" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E180" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F180" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="G180" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="H180" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="I180" s="41" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C181" s="37" t="s">
+      <c r="D182" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="E182" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F182" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="G182" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H182" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="I182" s="40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C183" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="D181" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E181" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F181" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="G181" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H181" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I181" s="41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C182" s="37" t="s">
-        <v>202</v>
-      </c>
-      <c r="D182" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E182" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F182" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="G182" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H182" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="I182" s="41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C183" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="D183" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="E183" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="F183" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="G183" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="H183" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="I183" s="45" t="s">
-        <v>175</v>
+      <c r="D183" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E183" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F183" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="G183" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="H183" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="I183" s="44" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="186" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B186" s="11"/>
-      <c r="C186" s="38" t="s">
+      <c r="C186" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="D186" s="37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="187" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C187" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="D186" s="38" t="s">
+      <c r="D187" s="38" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="187" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C187" s="37" t="s">
+    <row r="188" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C188" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="D187" s="39" t="s">
+      <c r="D188" s="38" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="188" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C188" s="37" t="s">
+    <row r="189" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C189" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="D188" s="39" t="s">
+      <c r="D189" s="38" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="189" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C189" s="37" t="s">
+    <row r="190" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C190" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="D189" s="39" t="s">
+      <c r="D190" s="38" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="190" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C190" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="D190" s="39" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="193" spans="2:4" ht="92.25" x14ac:dyDescent="0.4">
       <c r="B193" s="11">
         <v>45852</v>
       </c>
-      <c r="C193" s="47" t="s">
+      <c r="C193" s="46" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C194" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="D194" s="46"/>
+    </row>
+    <row r="196" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C196" s="46" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="194" spans="2:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="C194" s="47" t="s">
+    <row r="197" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C197" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="D194" s="47"/>
-    </row>
-    <row r="196" spans="2:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="C196" s="47" t="s">
+    </row>
+    <row r="198" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C198" s="46" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="197" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C197" s="47" t="s">
+    <row r="199" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C199" s="46" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="198" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C198" s="47" t="s">
+    <row r="200" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C200" s="46" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="199" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C199" s="47" t="s">
+    <row r="201" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C201" s="46" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="200" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C200" s="47" t="s">
+    <row r="202" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C202" s="46" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="201" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C201" s="47" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="202" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C202" s="47" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="204" spans="2:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B204" s="11">
         <v>45853</v>
       </c>
-      <c r="C204" s="48" t="s">
+      <c r="C204" s="47" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C205" s="48"/>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C206" s="49" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C207" s="48"/>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C208" s="49" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C205" s="49"/>
-    </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C206" s="50" t="s">
+    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C209" s="48"/>
+    </row>
+    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C210" s="49" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C207" s="49"/>
-    </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C208" s="50" t="s">
+    <row r="211" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C211" s="48"/>
+    </row>
+    <row r="212" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C212" s="49" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C209" s="49"/>
-    </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C210" s="50" t="s">
+    <row r="213" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C213" s="48"/>
+    </row>
+    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C214" s="49" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="211" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C211" s="49"/>
-    </row>
-    <row r="212" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C212" s="50" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="213" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C213" s="49"/>
-    </row>
-    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C214" s="50" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="217" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B217" s="11">
         <v>45857</v>
       </c>
-      <c r="C217" s="73" t="s">
+      <c r="C217" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="D217" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="E217" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="G217" s="51" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C218" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="D218" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="E218" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G218"/>
+    </row>
+    <row r="219" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C219" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="D219" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="E219" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="G219" s="52" t="s">
         <v>243</v>
       </c>
-      <c r="D217" s="38" t="s">
-        <v>234</v>
-      </c>
-      <c r="E217" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="G217" s="74" t="s">
+    </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C220" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="D220" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="E220" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="G220" s="48"/>
+    </row>
+    <row r="221" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C221" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="D221" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="E221" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="G221" s="48" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C218" s="39" t="s">
-        <v>236</v>
-      </c>
-      <c r="D218" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="E218" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="G218"/>
-    </row>
-    <row r="219" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C219" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="D219" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="E219" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="G219" s="75" t="s">
+    <row r="222" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G222" s="48"/>
+    </row>
+    <row r="223" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G223" s="48" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C220" s="39" t="s">
-        <v>238</v>
-      </c>
-      <c r="D220" s="39" t="s">
-        <v>239</v>
-      </c>
-      <c r="E220" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="G220" s="49"/>
-    </row>
-    <row r="221" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C221" s="39" t="s">
-        <v>240</v>
-      </c>
-      <c r="D221" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="E221" s="39" t="s">
-        <v>242</v>
-      </c>
-      <c r="G221" s="49" t="s">
+    <row r="224" spans="2:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="C224" s="53" t="s">
+        <v>252</v>
+      </c>
+      <c r="G224" s="48"/>
+    </row>
+    <row r="225" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C225" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G225" s="48" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="222" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G222" s="49"/>
-    </row>
-    <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G223" s="49" t="s">
+    <row r="226" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C226" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="G226"/>
+    </row>
+    <row r="227" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G227" s="52" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="224" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G224" s="49"/>
-    </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G225" s="49" t="s">
+    <row r="228" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G228" s="48"/>
+    </row>
+    <row r="229" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G229" s="48" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G226"/>
-    </row>
-    <row r="227" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G227" s="75" t="s">
+    <row r="230" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G230" s="48"/>
+    </row>
+    <row r="231" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G231" s="48" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G228" s="49"/>
-    </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G229" s="49" t="s">
+    <row r="232" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G232" s="48"/>
+    </row>
+    <row r="233" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G233" s="48" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G230" s="49"/>
-    </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G231" s="49" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G232" s="49"/>
-    </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G233" s="49" t="s">
-        <v>252</v>
+    <row r="244" spans="3:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="C244" s="51" t="s">
+        <v>256</v>
+      </c>
+      <c r="E244" s="51" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="245" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C245" s="48"/>
+      <c r="E245" s="48"/>
+    </row>
+    <row r="246" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C246" s="48" t="s">
+        <v>257</v>
+      </c>
+      <c r="E246" s="48" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="247" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C247" s="48"/>
+      <c r="E247" s="48"/>
+    </row>
+    <row r="248" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C248" s="48" t="s">
+        <v>258</v>
+      </c>
+      <c r="E248" s="48" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="249" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C249" s="48"/>
+      <c r="E249" s="48"/>
+    </row>
+    <row r="250" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C250" s="48" t="s">
+        <v>259</v>
+      </c>
+      <c r="E250" s="48" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GĐ 2-1-2: Triển khai hệ thống thông báo bằng Laravel Notifications; cập nhật chức năng tìm kiếm global user, project, task.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E0FC3D-D6B5-405A-A5CA-3F2184EBAB04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62BDAFA-E81C-47A8-8F3F-289BBB5C8F6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="266">
   <si>
     <t>STT</t>
   </si>
@@ -1353,6 +1353,14 @@
   </si>
   <si>
     <t>Policy kiểm soát “ai được làm gì trên đối tượng nào” (ví dụ: ai được xem, sửa, xóa một Project).</t>
+  </si>
+  <si>
+    <t>Tạo notification</t>
+  </si>
+  <si>
+    <t>B1: cấu hình  php artisan notifications:table
+php artisan migrate
+B2: tạo mới php artisan make:notification TaskAssigned</t>
   </si>
 </sst>
 </file>
@@ -1620,7 +1628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1756,6 +1764,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1774,53 +1830,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2414,10 +2434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K20"/>
+  <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2436,31 +2456,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="62"/>
+      <c r="E3" s="56"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="62"/>
+      <c r="E4" s="56"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2468,12 +2488,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="63" t="s">
+      <c r="H5" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2511,19 +2531,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="65">
+      <c r="A7" s="59">
         <v>1</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="71" t="s">
+      <c r="E7" s="65" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="21"/>
@@ -2540,11 +2560,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="72"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="66"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2561,11 +2581,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="72"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="66"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -2582,11 +2602,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="72"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="66"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -2601,11 +2621,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="72"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="66"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -2622,11 +2642,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="73"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="67"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -2641,19 +2661,19 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="55">
+      <c r="A13" s="71">
         <v>2</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="75" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="21"/>
@@ -2670,50 +2690,48 @@
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="60"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
         <v>230</v>
       </c>
       <c r="I14" s="25">
         <v>45856</v>
       </c>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>3</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="28"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="76"/>
+      <c r="H15" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="I15" s="25">
+        <v>45861</v>
+      </c>
+      <c r="J15" s="80" t="s">
+        <v>265</v>
+      </c>
       <c r="K15" s="29"/>
     </row>
     <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -2728,16 +2746,16 @@
     </row>
     <row r="17" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>25</v>
@@ -2749,16 +2767,16 @@
     </row>
     <row r="18" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>25</v>
@@ -2768,32 +2786,58 @@
       <c r="J18" s="28"/>
       <c r="K18" s="29"/>
     </row>
-    <row r="19" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="30"/>
+      <c r="H19" s="27"/>
       <c r="I19" s="25"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="9"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>7</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="30"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="32"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -2803,13 +2847,8 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
   </mergeCells>
-  <conditionalFormatting sqref="E15:E1048576 E1:E13">
+  <conditionalFormatting sqref="E16:E1048576 E1:E14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$G$6</formula>
     </cfRule>
@@ -2826,7 +2865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
   <dimension ref="B4:P250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A201" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F180" sqref="F180"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GĐ 3-2: Hoàn thiện các trang còn lại của User (create, show, recycle); cập nhật các chức năng liên quan như xác nhận mật khẩu, soft delete và force delete. Cột 'status' trong bảng users hiện chưa sử dụng, sẽ được triển khai ở các giai đoạn phát triển sau.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF42F0BC-C870-4462-92BB-4D13B0D8C32A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EBCB24-EFBF-4ED5-B807-66B9FD452B5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="262">
   <si>
     <t>STT</t>
   </si>
@@ -1103,16 +1103,7 @@
     <t>Gửi mail xác minh</t>
   </si>
   <si>
-    <t>Cần đăng nhập thủ công</t>
-  </si>
-  <si>
-    <t>✅ (email + password)</t>
-  </si>
-  <si>
     <t>Click link xác minh email</t>
-  </si>
-  <si>
-    <t>✅ → login thủ công</t>
   </si>
   <si>
     <t>✅ → login tự động luôn</t>
@@ -2139,6 +2130,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>252</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>5197393</xdr:colOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>105561</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECD29D12-8C94-48BD-A195-56A53636E9DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1692088" y="54875206"/>
+          <a:ext cx="8783276" cy="5630061"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>661147</xdr:colOff>
+      <xdr:row>255</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1652531</xdr:colOff>
+      <xdr:row>266</xdr:row>
+      <xdr:rowOff>112351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3193DD6D-FB5D-4B86-8B96-A66BB9C46F01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11149853" y="55558765"/>
+          <a:ext cx="9631119" cy="2095792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2429,26 +2508,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.109375" style="8"/>
-    <col min="8" max="8" width="32.6640625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="70.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="110.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="8"/>
+    <col min="1" max="1" width="5.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="8"/>
+    <col min="8" max="8" width="32.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="70.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="110.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
         <v>14</v>
       </c>
@@ -2457,7 +2536,7 @@
       <c r="D2" s="65"/>
       <c r="E2" s="65"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2466,7 +2545,7 @@
       </c>
       <c r="E3" s="66"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2475,7 +2554,7 @@
       </c>
       <c r="E4" s="66"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2488,7 +2567,7 @@
       <c r="J5" s="68"/>
       <c r="K5" s="68"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -2523,7 +2602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="69">
         <v>1</v>
       </c>
@@ -2531,10 +2610,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="78" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D7" s="72" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E7" s="75" t="s">
         <v>18</v>
@@ -2552,7 +2631,7 @@
       </c>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="70"/>
       <c r="B8" s="73"/>
       <c r="C8" s="79"/>
@@ -2573,7 +2652,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="70"/>
       <c r="B9" s="73"/>
       <c r="C9" s="79"/>
@@ -2594,7 +2673,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="70"/>
       <c r="B10" s="73"/>
       <c r="C10" s="79"/>
@@ -2613,7 +2692,7 @@
       </c>
       <c r="K10" s="26"/>
     </row>
-    <row r="11" spans="1:11" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="70"/>
       <c r="B11" s="73"/>
       <c r="C11" s="79"/>
@@ -2628,13 +2707,13 @@
         <v>45845</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="71"/>
       <c r="B12" s="74"/>
       <c r="C12" s="80"/>
@@ -2653,7 +2732,7 @@
       </c>
       <c r="K12" s="26"/>
     </row>
-    <row r="13" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="56">
         <v>2</v>
       </c>
@@ -2682,7 +2761,7 @@
       </c>
       <c r="K13" s="26"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="57"/>
       <c r="B14" s="57"/>
       <c r="C14" s="60"/>
@@ -2699,24 +2778,24 @@
       <c r="J14" s="34"/>
       <c r="K14" s="26"/>
     </row>
-    <row r="15" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="58"/>
       <c r="B15" s="58"/>
       <c r="C15" s="61"/>
       <c r="D15" s="58"/>
       <c r="E15" s="64"/>
       <c r="H15" s="27" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I15" s="25">
         <v>45861</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="K15" s="29"/>
     </row>
-    <row r="16" spans="1:11" ht="44.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -2724,10 +2803,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>260</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>18</v>
@@ -2737,7 +2816,7 @@
       <c r="J16" s="28"/>
       <c r="K16" s="29"/>
     </row>
-    <row r="17" spans="1:11" ht="44.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>4</v>
       </c>
@@ -2745,10 +2824,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>18</v>
@@ -2758,7 +2837,7 @@
       <c r="J17" s="28"/>
       <c r="K17" s="29"/>
     </row>
-    <row r="18" spans="1:11" ht="44.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>5</v>
       </c>
@@ -2766,10 +2845,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>18</v>
@@ -2779,7 +2858,7 @@
       <c r="J18" s="28"/>
       <c r="K18" s="29"/>
     </row>
-    <row r="19" spans="1:11" ht="44.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>6</v>
       </c>
@@ -2787,10 +2866,10 @@
         <v>12</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>18</v>
@@ -2800,7 +2879,7 @@
       <c r="J19" s="28"/>
       <c r="K19" s="29"/>
     </row>
-    <row r="20" spans="1:11" ht="44.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>7</v>
       </c>
@@ -2811,7 +2890,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>18</v>
@@ -2821,7 +2900,7 @@
       <c r="J20" s="31"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
     </row>
   </sheetData>
@@ -2858,357 +2937,357 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
   <dimension ref="B4:P250"/>
   <sheetViews>
-    <sheetView topLeftCell="A153" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E159" sqref="C159:E159"/>
+    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K176" sqref="K176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="13"/>
-    <col min="2" max="2" width="16.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="53.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.109375" style="13"/>
-    <col min="11" max="11" width="25.5546875" style="13" customWidth="1"/>
-    <col min="12" max="14" width="9.109375" style="13"/>
-    <col min="15" max="15" width="33.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="78.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="13"/>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="16.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.140625" style="13"/>
+    <col min="11" max="11" width="25.5703125" style="13" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="13"/>
+    <col min="15" max="15" width="33.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="78.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:15" s="19" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:15" s="19" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B4" s="11">
         <v>45843</v>
       </c>
       <c r="O4" s="20"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" s="13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="13" t="s">
         <v>41</v>
       </c>
       <c r="O24" s="16"/>
       <c r="P24" s="16"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="13" t="s">
         <v>42</v>
       </c>
       <c r="O25" s="16"/>
       <c r="P25" s="16"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C31" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C32" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="13" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C67" s="13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C68" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C69" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C70" s="13" t="s">
         <v>72</v>
       </c>
@@ -3216,7 +3295,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C71" s="13" t="s">
         <v>73</v>
       </c>
@@ -3230,7 +3309,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C72" s="13" t="s">
         <v>74</v>
       </c>
@@ -3244,7 +3323,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C73" s="13" t="s">
         <v>68</v>
       </c>
@@ -3258,7 +3337,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C74" s="13" t="s">
         <v>75</v>
       </c>
@@ -3272,7 +3351,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C75" s="13" t="s">
         <v>76</v>
       </c>
@@ -3286,7 +3365,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C76" s="13" t="s">
         <v>77</v>
       </c>
@@ -3300,7 +3379,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C77" s="13" t="s">
         <v>78</v>
       </c>
@@ -3314,7 +3393,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C78" s="13" t="s">
         <v>79</v>
       </c>
@@ -3328,7 +3407,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C79" s="13" t="s">
         <v>80</v>
       </c>
@@ -3342,7 +3421,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C80" s="13" t="s">
         <v>81</v>
       </c>
@@ -3356,260 +3435,260 @@
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="13" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="13" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C97" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C98" s="13" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C99" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C100" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C101" s="13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C102" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C103" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C104" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C105" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C106" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C107" s="13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="108" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B108" s="14"/>
       <c r="C108" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C109" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C110" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C111" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C112" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C113" s="13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C114" s="13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C115" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C116" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C117" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C118" s="13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C119" s="13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C120" s="13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C121" s="13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C122" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C123" s="13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="124" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C124" s="13" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C125" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C126" s="13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C127" s="13" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="128" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="16" t="s">
         <v>125</v>
       </c>
       <c r="D128" s="16"/>
     </row>
-    <row r="129" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C129" s="16" t="s">
         <v>126</v>
       </c>
       <c r="D129" s="16"/>
     </row>
-    <row r="130" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C130" s="13" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="131" spans="2:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="131" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B131" s="11">
         <v>45845</v>
       </c>
     </row>
-    <row r="143" spans="2:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="143" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B143" s="14"/>
       <c r="E143" s="17"/>
       <c r="F143" s="17"/>
@@ -3620,7 +3699,7 @@
       <c r="K143" s="17"/>
       <c r="L143" s="17"/>
     </row>
-    <row r="144" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E144" s="18"/>
       <c r="F144" s="18"/>
       <c r="G144" s="18"/>
@@ -3630,7 +3709,7 @@
       <c r="K144" s="18"/>
       <c r="L144" s="18"/>
     </row>
-    <row r="145" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E145" s="18"/>
       <c r="F145" s="18"/>
       <c r="G145" s="18"/>
@@ -3640,7 +3719,7 @@
       <c r="K145" s="18"/>
       <c r="L145" s="18"/>
     </row>
-    <row r="146" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E146" s="18"/>
       <c r="F146" s="18"/>
       <c r="G146" s="18"/>
@@ -3650,7 +3729,7 @@
       <c r="K146" s="18"/>
       <c r="L146" s="18"/>
     </row>
-    <row r="147" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E147" s="18"/>
       <c r="F147" s="18"/>
       <c r="G147" s="18"/>
@@ -3660,7 +3739,7 @@
       <c r="K147" s="18"/>
       <c r="L147" s="18"/>
     </row>
-    <row r="148" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E148" s="18"/>
       <c r="F148" s="18"/>
       <c r="G148" s="18"/>
@@ -3670,7 +3749,7 @@
       <c r="K148" s="18"/>
       <c r="L148" s="18"/>
     </row>
-    <row r="149" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E149" s="18"/>
       <c r="F149" s="18"/>
       <c r="G149" s="18"/>
@@ -3680,7 +3759,7 @@
       <c r="K149" s="18"/>
       <c r="L149" s="18"/>
     </row>
-    <row r="150" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E150" s="18"/>
       <c r="F150" s="18"/>
       <c r="G150" s="18"/>
@@ -3690,7 +3769,7 @@
       <c r="K150" s="18"/>
       <c r="L150" s="18"/>
     </row>
-    <row r="151" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E151" s="18"/>
       <c r="F151" s="18"/>
       <c r="G151" s="18"/>
@@ -3700,7 +3779,7 @@
       <c r="K151" s="18"/>
       <c r="L151" s="18"/>
     </row>
-    <row r="152" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E152" s="18"/>
       <c r="F152" s="18"/>
       <c r="G152" s="18"/>
@@ -3710,7 +3789,7 @@
       <c r="K152" s="18"/>
       <c r="L152" s="18"/>
     </row>
-    <row r="153" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E153" s="18"/>
       <c r="F153" s="18"/>
       <c r="G153" s="18"/>
@@ -3720,7 +3799,7 @@
       <c r="K153" s="18"/>
       <c r="L153" s="18"/>
     </row>
-    <row r="154" spans="2:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="154" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B154" s="11">
         <v>45851</v>
       </c>
@@ -3735,7 +3814,7 @@
       <c r="K154" s="18"/>
       <c r="L154" s="18"/>
     </row>
-    <row r="155" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C155" s="37" t="s">
         <v>133</v>
       </c>
@@ -3764,7 +3843,7 @@
       </c>
       <c r="L155" s="18"/>
     </row>
-    <row r="156" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C156" s="41" t="s">
         <v>165</v>
       </c>
@@ -3790,7 +3869,7 @@
       <c r="K156" s="18"/>
       <c r="L156" s="18"/>
     </row>
-    <row r="157" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C157" s="41" t="s">
         <v>166</v>
       </c>
@@ -3816,7 +3895,7 @@
       <c r="K157" s="18"/>
       <c r="L157" s="18"/>
     </row>
-    <row r="158" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C158" s="36" t="s">
         <v>167</v>
       </c>
@@ -3842,7 +3921,7 @@
       <c r="K158" s="18"/>
       <c r="L158" s="18"/>
     </row>
-    <row r="159" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C159" s="36" t="s">
         <v>168</v>
       </c>
@@ -3868,7 +3947,7 @@
       <c r="K159" s="18"/>
       <c r="L159" s="18"/>
     </row>
-    <row r="160" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C160" s="36" t="s">
         <v>169</v>
       </c>
@@ -3894,7 +3973,7 @@
       <c r="K160" s="18"/>
       <c r="L160" s="18"/>
     </row>
-    <row r="161" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C161" s="36" t="s">
         <v>170</v>
       </c>
@@ -3920,7 +3999,7 @@
       <c r="K161" s="18"/>
       <c r="L161" s="18"/>
     </row>
-    <row r="162" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C162" s="43" t="s">
         <v>171</v>
       </c>
@@ -3946,7 +4025,7 @@
       <c r="K162" s="18"/>
       <c r="L162" s="18"/>
     </row>
-    <row r="163" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C163" s="36" t="s">
         <v>172</v>
       </c>
@@ -3974,7 +4053,7 @@
       <c r="K163" s="18"/>
       <c r="L163" s="18"/>
     </row>
-    <row r="164" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C164" s="41" t="s">
         <v>173</v>
       </c>
@@ -3998,7 +4077,7 @@
       </c>
       <c r="J164" s="39"/>
     </row>
-    <row r="165" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C165" s="36" t="s">
         <v>174</v>
       </c>
@@ -4022,7 +4101,7 @@
       </c>
       <c r="J165" s="39"/>
     </row>
-    <row r="166" spans="2:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="166" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B166" s="14"/>
       <c r="C166" s="36" t="s">
         <v>175</v>
@@ -4047,7 +4126,7 @@
       </c>
       <c r="J166" s="39"/>
     </row>
-    <row r="167" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C167" s="36" t="s">
         <v>176</v>
       </c>
@@ -4071,7 +4150,7 @@
       </c>
       <c r="J167" s="39"/>
     </row>
-    <row r="168" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C168" s="36" t="s">
         <v>177</v>
       </c>
@@ -4095,7 +4174,7 @@
       </c>
       <c r="J168" s="39"/>
     </row>
-    <row r="169" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C169" s="43" t="s">
         <v>178</v>
       </c>
@@ -4119,7 +4198,7 @@
       </c>
       <c r="J169" s="39"/>
     </row>
-    <row r="170" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C170" s="36" t="s">
         <v>179</v>
       </c>
@@ -4143,7 +4222,7 @@
       </c>
       <c r="J170" s="39"/>
     </row>
-    <row r="171" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C171" s="41" t="s">
         <v>180</v>
       </c>
@@ -4167,7 +4246,7 @@
       </c>
       <c r="J171" s="39"/>
     </row>
-    <row r="172" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C172" s="36" t="s">
         <v>181</v>
       </c>
@@ -4191,7 +4270,7 @@
       </c>
       <c r="J172" s="39"/>
     </row>
-    <row r="173" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C173" s="36" t="s">
         <v>182</v>
       </c>
@@ -4215,7 +4294,7 @@
       </c>
       <c r="J173" s="38"/>
     </row>
-    <row r="174" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C174" s="36" t="s">
         <v>183</v>
       </c>
@@ -4239,7 +4318,7 @@
       </c>
       <c r="J174" s="38"/>
     </row>
-    <row r="175" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C175" s="36" t="s">
         <v>184</v>
       </c>
@@ -4263,7 +4342,7 @@
       </c>
       <c r="J175" s="38"/>
     </row>
-    <row r="176" spans="2:12" ht="15" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C176" s="43" t="s">
         <v>185</v>
       </c>
@@ -4286,7 +4365,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="177" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C177" s="36" t="s">
         <v>186</v>
       </c>
@@ -4309,7 +4388,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="178" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C178" s="41" t="s">
         <v>187</v>
       </c>
@@ -4332,7 +4411,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="179" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C179" s="36" t="s">
         <v>188</v>
       </c>
@@ -4355,7 +4434,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="180" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C180" s="36" t="s">
         <v>189</v>
       </c>
@@ -4378,7 +4457,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="181" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C181" s="36" t="s">
         <v>190</v>
       </c>
@@ -4401,7 +4480,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="182" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C182" s="36" t="s">
         <v>191</v>
       </c>
@@ -4424,7 +4503,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="183" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C183" s="43" t="s">
         <v>192</v>
       </c>
@@ -4447,7 +4526,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="186" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="186" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B186" s="11"/>
       <c r="C186" s="37" t="s">
         <v>195</v>
@@ -4456,7 +4535,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="187" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C187" s="36" t="s">
         <v>197</v>
       </c>
@@ -4464,7 +4543,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="188" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C188" s="36" t="s">
         <v>199</v>
       </c>
@@ -4472,7 +4551,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="189" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C189" s="36" t="s">
         <v>201</v>
       </c>
@@ -4480,7 +4559,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="190" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C190" s="36" t="s">
         <v>203</v>
       </c>
@@ -4488,7 +4567,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="193" spans="2:4" ht="88.8" x14ac:dyDescent="0.5">
+    <row r="193" spans="2:4" ht="92.25" x14ac:dyDescent="0.4">
       <c r="B193" s="11">
         <v>45852</v>
       </c>
@@ -4496,48 +4575,48 @@
         <v>205</v>
       </c>
     </row>
-    <row r="194" spans="2:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="C194" s="46" t="s">
         <v>206</v>
       </c>
       <c r="D194" s="46"/>
     </row>
-    <row r="196" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="C196" s="46" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="197" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C197" s="46" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="198" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="C198" s="46" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="199" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C199" s="46" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="200" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C200" s="46" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="201" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C201" s="46" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="202" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C202" s="46" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="204" spans="2:4" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="204" spans="2:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B204" s="11">
         <v>45853</v>
       </c>
@@ -4545,52 +4624,52 @@
         <v>214</v>
       </c>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C205" s="48"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C206" s="49" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C207" s="48"/>
     </row>
-    <row r="208" spans="2:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C208" s="49" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C209" s="48"/>
     </row>
-    <row r="210" spans="2:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C210" s="49" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="211" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C211" s="48"/>
     </row>
-    <row r="212" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C212" s="49" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="213" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C213" s="48"/>
     </row>
-    <row r="214" spans="2:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C214" s="49" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="217" spans="2:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="217" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B217" s="11">
         <v>45857</v>
       </c>
       <c r="C217" s="50" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D217" s="37" t="s">
         <v>223</v>
@@ -4599,10 +4678,10 @@
         <v>224</v>
       </c>
       <c r="G217" s="51" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C218" s="38" t="s">
         <v>225</v>
       </c>
@@ -4614,7 +4693,7 @@
       </c>
       <c r="G218"/>
     </row>
-    <row r="219" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C219" s="38" t="s">
         <v>226</v>
       </c>
@@ -4625,134 +4704,128 @@
         <v>163</v>
       </c>
       <c r="G219" s="52" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C220" s="38"/>
+      <c r="D220" s="38"/>
+      <c r="E220" s="38"/>
+      <c r="G220" s="48"/>
+    </row>
+    <row r="221" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C221" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="D221" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="E221" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="G221" s="48" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="222" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G222" s="48"/>
+    </row>
+    <row r="223" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G223" s="48" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="224" spans="2:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="C224" s="53" t="s">
+        <v>240</v>
+      </c>
+      <c r="G224" s="48"/>
+    </row>
+    <row r="225" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C225" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="G225" s="48" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="220" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C220" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="D220" s="38" t="s">
-        <v>228</v>
-      </c>
-      <c r="E220" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="G220" s="48"/>
-    </row>
-    <row r="221" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C221" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="D221" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="E221" s="38" t="s">
-        <v>231</v>
-      </c>
-      <c r="G221" s="48" t="s">
+    <row r="226" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C226" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="G226"/>
+    </row>
+    <row r="227" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G227" s="52" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="222" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G222" s="48"/>
-    </row>
-    <row r="223" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G223" s="48" t="s">
+    <row r="228" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G228" s="48"/>
+    </row>
+    <row r="229" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G229" s="48" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="224" spans="2:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="C224" s="53" t="s">
-        <v>243</v>
-      </c>
-      <c r="G224" s="48"/>
-    </row>
-    <row r="225" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C225" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="G225" s="48" t="s">
+    <row r="230" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G230" s="48"/>
+    </row>
+    <row r="231" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G231" s="48" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="226" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C226" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="G226"/>
-    </row>
-    <row r="227" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="G227" s="52" t="s">
+    <row r="232" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G232" s="48"/>
+    </row>
+    <row r="233" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G233" s="48" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="228" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G228" s="48"/>
-    </row>
-    <row r="229" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G229" s="48" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="230" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G230" s="48"/>
-    </row>
-    <row r="231" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G231" s="48" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="232" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G232" s="48"/>
-    </row>
-    <row r="233" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G233" s="48" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="244" spans="3:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="244" spans="3:5" ht="18" x14ac:dyDescent="0.25">
       <c r="C244" s="51" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E244" s="51" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="245" spans="3:5" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="245" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C245" s="48"/>
       <c r="E245" s="48"/>
     </row>
-    <row r="246" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C246" s="48" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E246" s="48" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="247" spans="3:5" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="247" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C247" s="48"/>
       <c r="E247" s="48"/>
     </row>
-    <row r="248" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C248" s="48" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E248" s="48" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="249" spans="3:5" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="249" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C249" s="48"/>
       <c r="E249" s="48"/>
     </row>
-    <row r="250" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C250" s="48" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E250" s="48" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GĐ 1-12-3: Cập nhật lại quyền của manager, leader, member, client.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EBCB24-EFBF-4ED5-B807-66B9FD452B5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996732D5-2895-46CC-AF70-8F62E353240E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1751,6 +1751,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1777,54 +1825,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2528,31 +2528,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="66"/>
+      <c r="E3" s="57"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="66"/>
+      <c r="E4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2560,12 +2560,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="67" t="s">
+      <c r="H5" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2603,19 +2603,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="69">
+      <c r="A7" s="60">
         <v>1</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="69" t="s">
         <v>255</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="63" t="s">
         <v>256</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="66" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="21"/>
@@ -2632,11 +2632,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="70"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="76"/>
+      <c r="A8" s="61"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="67"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2653,11 +2653,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="70"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="76"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="67"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -2674,11 +2674,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="76"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="67"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -2693,11 +2693,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
-      <c r="B11" s="73"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="76"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="67"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -2714,11 +2714,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="77"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="68"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -2733,19 +2733,19 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="56">
+      <c r="A13" s="72">
         <v>2</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="78" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="21"/>
@@ -2762,11 +2762,11 @@
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="63"/>
+      <c r="A14" s="73"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="79"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
@@ -2779,11 +2779,11 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="64"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="80"/>
       <c r="H15" s="27" t="s">
         <v>252</v>
       </c>
@@ -2905,6 +2905,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -2914,11 +2919,6 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1048576 E1:E14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -2938,7 +2938,7 @@
   <dimension ref="B4:P250"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A153" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K176" sqref="K176"/>
+      <selection activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3839,7 +3839,7 @@
       <c r="J155" s="33"/>
       <c r="K155">
         <f>COUNTIF(D156:I183, D156) + COUNTIF(D156:I183, F159)</f>
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="L155" s="18"/>
     </row>
@@ -4137,7 +4137,7 @@
         <v>163</v>
       </c>
       <c r="F167" s="40" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="G167" s="40" t="s">
         <v>164</v>
@@ -4161,7 +4161,7 @@
         <v>163</v>
       </c>
       <c r="F168" s="40" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="G168" s="40" t="s">
         <v>164</v>
@@ -4308,7 +4308,7 @@
         <v>163</v>
       </c>
       <c r="G174" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H174" s="40" t="s">
         <v>164</v>
@@ -4332,7 +4332,7 @@
         <v>163</v>
       </c>
       <c r="G175" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H175" s="40" t="s">
         <v>164</v>
@@ -4353,7 +4353,7 @@
         <v>163</v>
       </c>
       <c r="F176" s="44" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G176" s="44" t="s">
         <v>164</v>
@@ -4468,16 +4468,16 @@
         <v>163</v>
       </c>
       <c r="F181" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G181" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H181" s="40" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="I181" s="40" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.25">
@@ -4491,16 +4491,16 @@
         <v>163</v>
       </c>
       <c r="F182" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G182" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H182" s="40" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="I182" s="40" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
     </row>
     <row r="183" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
GĐ 4-1: Xây dựng giao diện quản lý projects.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996732D5-2895-46CC-AF70-8F62E353240E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64BBB58-0D34-4B3D-8892-EA93A88BF85D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="263">
   <si>
     <t>STT</t>
   </si>
@@ -1345,6 +1345,9 @@
   </si>
   <si>
     <t>4-5 ngày</t>
+  </si>
+  <si>
+    <t>Thêm hàm bên trên vào model để laravel lấy slug hiển thị trên url thay vì id :http://127.0.0.1:8000/projects/12</t>
   </si>
 </sst>
 </file>
@@ -2218,6 +2221,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1205861</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>57344</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FFF4818-937E-4008-9044-86C6CC970FBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1692088" y="60780706"/>
+          <a:ext cx="4791744" cy="1390844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1871382</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>380384</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>22492</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFB5B971-AE5F-46BB-90D8-D51432FB4D1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7149353" y="60803118"/>
+          <a:ext cx="7630590" cy="571580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2935,10 +3026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
-  <dimension ref="B4:P250"/>
+  <dimension ref="B4:P292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E186" sqref="E186"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K161" sqref="K161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4828,6 +4919,11 @@
         <v>251</v>
       </c>
     </row>
+    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C292" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GĐ 4-1-1: Gửi thông báo khi user được assign vào project. Dùng queue (tạo bảng jobs) để xử lý bất đồng bộ. Cập nhật APP_URL=http://127.0.0.1:8000 để thông báo trỏ đúng server. Chạy php artisan queue:work để kích hoạt xử lý hàng đợi.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64BBB58-0D34-4B3D-8892-EA93A88BF85D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC01A288-1272-41E3-BF9C-5E479F669234}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="264">
   <si>
     <t>STT</t>
   </si>
@@ -1348,6 +1348,11 @@
   </si>
   <si>
     <t>Thêm hàm bên trên vào model để laravel lấy slug hiển thị trên url thay vì id :http://127.0.0.1:8000/projects/12</t>
+  </si>
+  <si>
+    <t>dùng queque để thông báo bất đồng bộ (thông báo chỉ gửi sau khi commit, và đợi trong hàng chờ)
+php artisan queue:table -&gt; php artisan migrate
+khi demo nhớ chạy: php artisan queue:work</t>
   </si>
 </sst>
 </file>
@@ -1615,7 +1620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1754,6 +1759,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1802,32 +1834,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2599,8 +2607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2619,31 +2627,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="57"/>
+      <c r="E3" s="66"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="66"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2651,12 +2659,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="58" t="s">
+      <c r="H5" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2694,19 +2702,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="60">
+      <c r="A7" s="69">
         <v>1</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="78" t="s">
         <v>255</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="72" t="s">
         <v>256</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="75" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="21"/>
@@ -2723,11 +2731,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="67"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="76"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2744,11 +2752,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
-      <c r="B9" s="64"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="67"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="76"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -2765,11 +2773,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="67"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="76"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -2784,11 +2792,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="67"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="76"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -2805,11 +2813,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="68"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="77"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -2824,19 +2832,19 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="72">
+      <c r="A13" s="56">
         <v>2</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="78" t="s">
+      <c r="E13" s="62" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="21"/>
@@ -2853,11 +2861,11 @@
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="79"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="63"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
@@ -2870,11 +2878,11 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="80"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="64"/>
       <c r="H15" s="27" t="s">
         <v>252</v>
       </c>
@@ -2884,7 +2892,9 @@
       <c r="J15" s="55" t="s">
         <v>253</v>
       </c>
-      <c r="K15" s="29"/>
+      <c r="K15" s="81" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -2996,11 +3006,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -3010,6 +3015,11 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1048576 E1:E14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3028,7 +3038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
   <dimension ref="B4:P292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K161" sqref="K161"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GĐ 6-1: Tích hợp phần bình luận vào giao diện Task; thêm chức năng tạo bình luận mới; đang sửa lỗi phần chỉnh sửa bình luận.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC01A288-1272-41E3-BF9C-5E479F669234}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1639D7-10EB-4061-9611-8BAC4C1EEADB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="263">
   <si>
     <t>STT</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Quản lý dự án</t>
-  </si>
-  <si>
-    <t>Quản lý task</t>
   </si>
   <si>
     <t>Trao đổi trong task</t>
@@ -1759,6 +1756,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1833,9 +1833,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2108,7 +2105,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1430</xdr:colOff>
       <xdr:row>242</xdr:row>
-      <xdr:rowOff>183203</xdr:rowOff>
+      <xdr:rowOff>187013</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2149,10 +2146,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>5197393</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>328</xdr:colOff>
       <xdr:row>281</xdr:row>
-      <xdr:rowOff>105561</xdr:rowOff>
+      <xdr:rowOff>111276</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2194,7 +2191,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1652531</xdr:colOff>
+      <xdr:colOff>1643006</xdr:colOff>
       <xdr:row>266</xdr:row>
       <xdr:rowOff>112351</xdr:rowOff>
     </xdr:to>
@@ -2238,9 +2235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1205861</xdr:colOff>
+      <xdr:colOff>1215386</xdr:colOff>
       <xdr:row>290</xdr:row>
-      <xdr:rowOff>57344</xdr:rowOff>
+      <xdr:rowOff>72584</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2284,7 +2281,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>380384</xdr:colOff>
       <xdr:row>286</xdr:row>
-      <xdr:rowOff>22492</xdr:rowOff>
+      <xdr:rowOff>33922</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2607,8 +2604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2627,31 +2624,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="A2" s="66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="66"/>
+      <c r="D3" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="67"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="66"/>
+      <c r="D4" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2659,12 +2656,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
+      <c r="H5" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2683,193 +2680,193 @@
         <v>4</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="H6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="69">
+      <c r="A7" s="70">
         <v>1</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="79" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="73" t="s">
         <v>255</v>
       </c>
-      <c r="D7" s="72" t="s">
-        <v>256</v>
-      </c>
-      <c r="E7" s="75" t="s">
-        <v>18</v>
+      <c r="E7" s="76" t="s">
+        <v>17</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I7" s="23">
         <v>45843</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="70"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="76"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="77"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I8" s="25">
         <v>45843</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="70"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="76"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="77"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I9" s="25">
         <v>45844</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="76"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="77"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I10" s="25">
         <v>45845</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="70"/>
-      <c r="B11" s="73"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="76"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="77"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I11" s="25">
         <v>45845</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="77"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="78"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I12" s="25">
         <v>45851</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="56">
+      <c r="A13" s="57">
         <v>2</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="62" t="s">
-        <v>18</v>
+      <c r="E13" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I13" s="25">
         <v>45854</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="63"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="64"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I14" s="25">
         <v>45856</v>
@@ -2878,22 +2875,22 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="64"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="65"/>
       <c r="H15" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I15" s="25">
         <v>45861</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>253</v>
-      </c>
-      <c r="K15" s="81" t="s">
-        <v>263</v>
+        <v>252</v>
+      </c>
+      <c r="K15" s="56" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
@@ -2904,13 +2901,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" s="27"/>
       <c r="I16" s="25"/>
@@ -2925,13 +2922,13 @@
         <v>10</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H17" s="27"/>
       <c r="I17" s="25"/>
@@ -2943,16 +2940,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="25"/>
@@ -2964,16 +2961,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="25"/>
@@ -2985,16 +2982,16 @@
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H20" s="30"/>
       <c r="I20" s="25"/>
@@ -3038,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
   <dimension ref="B4:P292"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K161" sqref="K161"/>
+    <sheetView topLeftCell="C162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K180" sqref="K180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3066,722 +3063,722 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="3:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O24" s="16"/>
       <c r="P24" s="16"/>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O25" s="16"/>
       <c r="P25" s="16"/>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C31" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C32" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C67" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C68" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C69" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C70" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D70" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C71" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D71" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E71" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="E71" s="13" t="s">
+      <c r="F71" s="13" t="s">
         <v>139</v>
-      </c>
-      <c r="F71" s="13" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C72" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D72" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E72" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E72" s="13" t="s">
+      <c r="F72" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="F72" s="13" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C73" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E73" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F73" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="F73" s="13" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C74" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E74" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F74" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="F74" s="13" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C75" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E75" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F75" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="F75" s="13" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C76" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C77" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C78" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C79" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C80" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C97" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C98" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C99" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C100" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C101" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C102" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C103" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C104" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C105" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C106" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C107" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="108" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B108" s="14"/>
       <c r="C108" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C109" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C110" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C111" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C112" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C113" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="114" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C114" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C115" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C116" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="117" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C117" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="118" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C118" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="119" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C119" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="120" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C120" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="121" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C121" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="122" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C122" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="123" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C123" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="124" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C124" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="125" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C125" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C126" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="127" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C127" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="128" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C128" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D128" s="16"/>
     </row>
     <row r="129" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C129" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D129" s="16"/>
     </row>
     <row r="130" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C130" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="131" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
@@ -3917,25 +3914,25 @@
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C155" s="37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D155" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="E155" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="E155" s="37" t="s">
+      <c r="F155" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="F155" s="37" t="s">
+      <c r="G155" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="G155" s="37" t="s">
+      <c r="H155" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="H155" s="37" t="s">
+      <c r="I155" s="37" t="s">
         <v>161</v>
-      </c>
-      <c r="I155" s="37" t="s">
-        <v>162</v>
       </c>
       <c r="J155" s="33"/>
       <c r="K155">
@@ -3946,25 +3943,25 @@
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C156" s="41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D156" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E156" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F156" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G156" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H156" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I156" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J156" s="39"/>
       <c r="K156" s="18"/>
@@ -3972,25 +3969,25 @@
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C157" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D157" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E157" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F157" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G157" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H157" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I157" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J157" s="39"/>
       <c r="K157" s="18"/>
@@ -3998,25 +3995,25 @@
     </row>
     <row r="158" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C158" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D158" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E158" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F158" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G158" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H158" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I158" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J158" s="39"/>
       <c r="K158" s="18"/>
@@ -4024,25 +4021,25 @@
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C159" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D159" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E159" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F159" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G159" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H159" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I159" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J159" s="39"/>
       <c r="K159" s="18"/>
@@ -4050,25 +4047,25 @@
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C160" s="36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D160" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E160" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F160" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G160" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H160" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I160" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J160" s="39"/>
       <c r="K160" s="18"/>
@@ -4076,25 +4073,25 @@
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C161" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D161" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E161" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F161" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G161" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H161" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I161" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J161" s="39"/>
       <c r="K161" s="18"/>
@@ -4102,25 +4099,25 @@
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C162" s="43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D162" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E162" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F162" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G162" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H162" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I162" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J162" s="39"/>
       <c r="K162" s="18"/>
@@ -4128,544 +4125,544 @@
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C163" s="36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D163" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E163" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F163" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G163" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H163" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I163" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J163" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K163" s="18"/>
       <c r="L163" s="18"/>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C164" s="41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D164" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E164" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F164" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G164" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H164" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I164" s="42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J164" s="39"/>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C165" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D165" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E165" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F165" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G165" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H165" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I165" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J165" s="39"/>
     </row>
     <row r="166" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B166" s="14"/>
       <c r="C166" s="36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D166" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E166" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F166" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G166" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H166" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I166" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J166" s="39"/>
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C167" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D167" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E167" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F167" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G167" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H167" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I167" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J167" s="39"/>
     </row>
     <row r="168" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C168" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D168" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E168" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F168" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G168" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H168" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I168" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J168" s="39"/>
     </row>
     <row r="169" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C169" s="43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D169" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E169" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F169" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G169" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H169" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I169" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J169" s="39"/>
     </row>
     <row r="170" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C170" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D170" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E170" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F170" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G170" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H170" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I170" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J170" s="39"/>
     </row>
     <row r="171" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C171" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D171" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E171" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F171" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G171" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H171" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I171" s="42" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="J171" s="39"/>
     </row>
     <row r="172" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C172" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D172" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E172" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F172" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G172" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H172" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I172" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J172" s="39"/>
     </row>
     <row r="173" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C173" s="36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D173" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E173" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F173" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G173" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H173" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I173" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J173" s="38"/>
     </row>
     <row r="174" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C174" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D174" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E174" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F174" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G174" s="40" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="H174" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I174" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J174" s="38"/>
     </row>
     <row r="175" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C175" s="36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D175" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E175" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F175" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G175" s="40" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="H175" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I175" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J175" s="38"/>
     </row>
     <row r="176" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C176" s="43" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D176" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E176" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F176" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G176" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H176" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I176" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C177" s="36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D177" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E177" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F177" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G177" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H177" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I177" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C178" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D178" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E178" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F178" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G178" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H178" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I178" s="42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C179" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D179" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E179" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F179" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G179" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H179" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I179" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C180" s="36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D180" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E180" s="40" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="F180" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G180" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H180" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I180" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="181" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C181" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D181" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E181" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F181" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G181" s="40" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="H181" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I181" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C182" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D182" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E182" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F182" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G182" s="40" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="H182" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I182" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="183" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C183" s="43" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D183" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E183" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F183" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G183" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H183" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I183" s="44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="186" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B186" s="11"/>
       <c r="C186" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="D186" s="37" t="s">
         <v>195</v>
-      </c>
-      <c r="D186" s="37" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="187" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C187" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="D187" s="38" t="s">
         <v>197</v>
-      </c>
-      <c r="D187" s="38" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="188" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C188" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="D188" s="38" t="s">
         <v>199</v>
-      </c>
-      <c r="D188" s="38" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="189" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C189" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="D189" s="38" t="s">
         <v>201</v>
-      </c>
-      <c r="D189" s="38" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="190" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C190" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="D190" s="38" t="s">
         <v>203</v>
-      </c>
-      <c r="D190" s="38" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="193" spans="2:4" ht="92.25" x14ac:dyDescent="0.4">
@@ -4673,48 +4670,48 @@
         <v>45852</v>
       </c>
       <c r="C193" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="194" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="C194" s="46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D194" s="46"/>
     </row>
     <row r="196" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="C196" s="46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="197" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C197" s="46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="198" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="C198" s="46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="199" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C199" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="200" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C200" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="201" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C201" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="202" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C202" s="46" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="204" spans="2:4" ht="26.25" x14ac:dyDescent="0.4">
@@ -4722,7 +4719,7 @@
         <v>45853</v>
       </c>
       <c r="C204" s="47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
@@ -4730,7 +4727,7 @@
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C206" s="49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
@@ -4738,7 +4735,7 @@
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C208" s="49" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="209" spans="2:7" x14ac:dyDescent="0.25">
@@ -4746,7 +4743,7 @@
     </row>
     <row r="210" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C210" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="211" spans="2:7" x14ac:dyDescent="0.25">
@@ -4754,7 +4751,7 @@
     </row>
     <row r="212" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C212" s="49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
@@ -4762,7 +4759,7 @@
     </row>
     <row r="214" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C214" s="49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="217" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
@@ -4770,42 +4767,42 @@
         <v>45857</v>
       </c>
       <c r="C217" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="D217" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="E217" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="G217" s="51" t="s">
         <v>229</v>
-      </c>
-      <c r="D217" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="E217" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="G217" s="51" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C218" s="38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D218" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E218" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G218"/>
     </row>
     <row r="219" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C219" s="38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D219" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E219" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G219" s="52" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="220" spans="2:7" x14ac:dyDescent="0.25">
@@ -4816,16 +4813,16 @@
     </row>
     <row r="221" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C221" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="D221" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="D221" s="38" t="s">
-        <v>228</v>
-      </c>
       <c r="E221" s="38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G221" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="222" spans="2:7" x14ac:dyDescent="0.25">
@@ -4833,32 +4830,32 @@
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G223" s="48" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="224" spans="2:7" ht="21" x14ac:dyDescent="0.35">
       <c r="C224" s="53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G224" s="48"/>
     </row>
     <row r="225" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C225" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G225" s="48" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="226" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C226" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G226"/>
     </row>
     <row r="227" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G227" s="52" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="228" spans="3:7" x14ac:dyDescent="0.25">
@@ -4866,7 +4863,7 @@
     </row>
     <row r="229" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G229" s="48" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="230" spans="3:7" x14ac:dyDescent="0.25">
@@ -4874,7 +4871,7 @@
     </row>
     <row r="231" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G231" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="232" spans="3:7" x14ac:dyDescent="0.25">
@@ -4882,15 +4879,15 @@
     </row>
     <row r="233" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G233" s="48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="244" spans="3:5" ht="18" x14ac:dyDescent="0.25">
       <c r="C244" s="51" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E244" s="51" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="245" spans="3:5" x14ac:dyDescent="0.25">
@@ -4899,10 +4896,10 @@
     </row>
     <row r="246" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C246" s="48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E246" s="48" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="247" spans="3:5" x14ac:dyDescent="0.25">
@@ -4911,10 +4908,10 @@
     </row>
     <row r="248" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C248" s="48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E248" s="48" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="249" spans="3:5" x14ac:dyDescent="0.25">
@@ -4923,15 +4920,15 @@
     </row>
     <row r="250" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C250" s="48" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E250" s="48" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="292" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C292" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GĐ 6-2: Thiết kế giao diện danh sách và thùng rác bình luận (recycle); Bỏ viewAny trong TaskPolicy (không còn cần thiết); Khi truy cập task từ thông báo bình luận, tự động cuộn và làm nổi bật bình luận tương ứng.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1639D7-10EB-4061-9611-8BAC4C1EEADB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E62FFC-623B-4709-AF85-3E07555ED284}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -1759,6 +1759,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1785,54 +1833,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2604,7 +2604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -2624,31 +2624,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="67"/>
+      <c r="E3" s="58"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="58"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2656,12 +2656,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="68" t="s">
+      <c r="H5" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2699,19 +2699,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="70">
+      <c r="A7" s="61">
         <v>1</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="70" t="s">
         <v>254</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="64" t="s">
         <v>255</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="67" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="21"/>
@@ -2728,11 +2728,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="77"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="68"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2749,11 +2749,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="77"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -2770,11 +2770,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="77"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -2789,11 +2789,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="77"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="68"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -2810,11 +2810,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="78"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="69"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -2829,19 +2829,19 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="57">
+      <c r="A13" s="73">
         <v>2</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="57" t="s">
+      <c r="D13" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="79" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="21"/>
@@ -2858,11 +2858,11 @@
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="64"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="80"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
@@ -2875,11 +2875,11 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="65"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="81"/>
       <c r="H15" s="27" t="s">
         <v>251</v>
       </c>
@@ -3003,6 +3003,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -3012,11 +3017,6 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1048576 E1:E14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3035,7 +3035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
   <dimension ref="B4:P292"/>
   <sheetViews>
-    <sheetView topLeftCell="C162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K180" sqref="K180"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GĐ 7-1: Tạo bảng files; khởi tạo controller, model, policy, service, view, và route cho file; cập nhật permission liên quan.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E62FFC-623B-4709-AF85-3E07555ED284}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECF1F1C-E766-4C4D-B4E1-541FDA632541}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="306">
   <si>
     <t>STT</t>
   </si>
@@ -540,9 +540,6 @@
     <t>user.force-delete</t>
   </si>
   <si>
-    <t>user.assign</t>
-  </si>
-  <si>
     <t>project.view</t>
   </si>
   <si>
@@ -561,9 +558,6 @@
     <t>project.force-delete</t>
   </si>
   <si>
-    <t>project.assign</t>
-  </si>
-  <si>
     <t>task.view</t>
   </si>
   <si>
@@ -582,9 +576,6 @@
     <t>task.force-delete</t>
   </si>
   <si>
-    <t>task.assign</t>
-  </si>
-  <si>
     <t>comment.view</t>
   </si>
   <si>
@@ -604,9 +595,6 @@
   </si>
   <si>
     <t>✅own</t>
-  </si>
-  <si>
-    <t>gán role</t>
   </si>
   <si>
     <t>Tình huống</t>
@@ -1350,6 +1338,147 @@
     <t>dùng queque để thông báo bất đồng bộ (thông báo chỉ gửi sau khi commit, và đợi trong hàng chờ)
 php artisan queue:table -&gt; php artisan migrate
 khi demo nhớ chạy: php artisan queue:work</t>
+  </si>
+  <si>
+    <t>Loại hành động</t>
+  </si>
+  <si>
+    <t>Nội dung thông báo mẫu</t>
+  </si>
+  <si>
+    <t>Ai nhận?</t>
+  </si>
+  <si>
+    <t>Tạo mới (Create)</t>
+  </si>
+  <si>
+    <t>"Bạn được giao task mới: [Tên task]"</t>
+  </si>
+  <si>
+    <t>Người được gán task, creator</t>
+  </si>
+  <si>
+    <t>Thông báo phổ biến nhất</t>
+  </si>
+  <si>
+    <t>Cập nhật (Update)</t>
+  </si>
+  <si>
+    <t>"Task '[Tên task]' đã chuyển trạng thái thành [Trạng thái mới]"</t>
+  </si>
+  <si>
+    <t>Người theo dõi task, assign</t>
+  </si>
+  <si>
+    <t>Thay đổi trạng thái, deadline...</t>
+  </si>
+  <si>
+    <t>Comment mới</t>
+  </si>
+  <si>
+    <t>"[Người comment] đã comment vào task '[Tên task]'"</t>
+  </si>
+  <si>
+    <t>Người theo dõi, người được mention</t>
+  </si>
+  <si>
+    <t>Thường kèm mention nếu có</t>
+  </si>
+  <si>
+    <t>Mention</t>
+  </si>
+  <si>
+    <t>"Bạn được mention trong comment task '[Tên task]'"</t>
+  </si>
+  <si>
+    <t>Người được mention</t>
+  </si>
+  <si>
+    <t>Quan trọng, tạo sự chú ý</t>
+  </si>
+  <si>
+    <t>Thêm vào Project</t>
+  </si>
+  <si>
+    <t>"Bạn được thêm vào project '[Tên project]'"</t>
+  </si>
+  <si>
+    <t>Người được thêm</t>
+  </si>
+  <si>
+    <t>Khi user mới tham gia project</t>
+  </si>
+  <si>
+    <t>Deadline sắp đến</t>
+  </si>
+  <si>
+    <t>"Task '[Tên task]' sắp đến deadline (còn X ngày)"</t>
+  </si>
+  <si>
+    <t>Người được giao task</t>
+  </si>
+  <si>
+    <t>Cảnh báo quan trọng</t>
+  </si>
+  <si>
+    <t>Restore</t>
+  </si>
+  <si>
+    <t>"Task '[Tên task]' đã được khôi phục"</t>
+  </si>
+  <si>
+    <t>Người được giao, creator, admin</t>
+  </si>
+  <si>
+    <t>Khi khôi phục từ soft delete</t>
+  </si>
+  <si>
+    <t>Force Delete</t>
+  </si>
+  <si>
+    <t>"Task '[Tên task]' đã bị xóa vĩnh viễn bởi [Người thực hiện]"</t>
+  </si>
+  <si>
+    <t>Người liên quan trực tiếp</t>
+  </si>
+  <si>
+    <t>Khi xóa vĩnh viễn (tuỳ trường hợp)</t>
+  </si>
+  <si>
+    <t>Xóa (Soft Delete)</t>
+  </si>
+  <si>
+    <t>"Task '[Tên task]' đã bị xóa"</t>
+  </si>
+  <si>
+    <t>Người được giao, creator</t>
+  </si>
+  <si>
+    <t>Khi soft delete, có thể hoặc không gửi</t>
+  </si>
+  <si>
+    <t>file.view</t>
+  </si>
+  <si>
+    <t>file.soft-delete</t>
+  </si>
+  <si>
+    <t>file.restore</t>
+  </si>
+  <si>
+    <t>file.force-delete</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>file.upload</t>
+  </si>
+  <si>
+    <t>file.dowload</t>
+  </si>
+  <si>
+    <t>File</t>
   </si>
 </sst>
 </file>
@@ -1508,7 +1637,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1613,11 +1742,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1759,6 +1901,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1807,31 +1976,16 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1927,7 +2081,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>530125</xdr:colOff>
+      <xdr:colOff>537745</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>73244</xdr:rowOff>
     </xdr:to>
@@ -2098,14 +2252,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>134471</xdr:colOff>
-      <xdr:row>226</xdr:row>
+      <xdr:row>232</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1430</xdr:colOff>
-      <xdr:row>242</xdr:row>
-      <xdr:rowOff>187013</xdr:rowOff>
+      <xdr:row>249</xdr:row>
+      <xdr:rowOff>4469</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2142,13 +2296,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>252</xdr:row>
+      <xdr:row>258</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>328</xdr:colOff>
-      <xdr:row>281</xdr:row>
+      <xdr:row>287</xdr:row>
       <xdr:rowOff>111276</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2186,13 +2340,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>661147</xdr:colOff>
-      <xdr:row>255</xdr:row>
+      <xdr:row>261</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>1643006</xdr:colOff>
-      <xdr:row>266</xdr:row>
+      <xdr:row>272</xdr:row>
       <xdr:rowOff>112351</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2230,13 +2384,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>283</xdr:row>
+      <xdr:row>289</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1215386</xdr:colOff>
-      <xdr:row>290</xdr:row>
+      <xdr:row>296</xdr:row>
       <xdr:rowOff>72584</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2274,13 +2428,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1871382</xdr:colOff>
-      <xdr:row>283</xdr:row>
+      <xdr:row>289</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>380384</xdr:colOff>
-      <xdr:row>286</xdr:row>
+      <xdr:colOff>378479</xdr:colOff>
+      <xdr:row>292</xdr:row>
       <xdr:rowOff>33922</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2602,10 +2756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K21"/>
+  <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2624,31 +2778,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="58"/>
+      <c r="E3" s="67"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="58"/>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2656,12 +2810,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2699,19 +2853,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="61">
+      <c r="A7" s="70">
         <v>1</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="70" t="s">
-        <v>254</v>
-      </c>
-      <c r="D7" s="64" t="s">
-        <v>255</v>
-      </c>
-      <c r="E7" s="67" t="s">
+      <c r="C7" s="79" t="s">
+        <v>250</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" s="76" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="21"/>
@@ -2728,11 +2882,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="68"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="77"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2749,11 +2903,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="68"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="77"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -2770,11 +2924,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="68"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="77"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -2789,11 +2943,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="68"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="77"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -2803,18 +2957,18 @@
         <v>45845</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="69"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="78"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -2829,44 +2983,44 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="73">
+      <c r="A13" s="57">
         <v>2</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="73" t="s">
+      <c r="D13" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="79" t="s">
+      <c r="E13" s="63" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="27" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I13" s="25">
         <v>45854</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="80"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="64"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I14" s="25">
         <v>45856</v>
@@ -2875,22 +3029,22 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="81"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="65"/>
       <c r="H15" s="27" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I15" s="25">
         <v>45861</v>
       </c>
       <c r="J15" s="55" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="K15" s="56" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
@@ -2901,10 +3055,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>17</v>
@@ -2922,10 +3076,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>17</v>
@@ -2943,10 +3097,10 @@
         <v>7</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>17</v>
@@ -2964,10 +3118,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>17</v>
@@ -2982,32 +3136,42 @@
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="7"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="85"/>
+    </row>
+    <row r="21" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>8</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="D21" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="32"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="9"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="32"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -3017,6 +3181,11 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1048576 E1:E14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3033,10 +3202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
-  <dimension ref="B4:P292"/>
+  <dimension ref="A4:P309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K180" sqref="K180"/>
+    <sheetView topLeftCell="A150" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,7 +3216,8 @@
     <col min="4" max="4" width="78.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="13" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" style="13"/>
+    <col min="7" max="9" width="9.140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="13"/>
     <col min="11" max="11" width="25.5703125" style="13" customWidth="1"/>
     <col min="12" max="14" width="9.140625" style="13"/>
     <col min="15" max="15" width="33.5703125" style="13" bestFit="1" customWidth="1"/>
@@ -3936,8 +4106,8 @@
       </c>
       <c r="J155" s="33"/>
       <c r="K155">
-        <f>COUNTIF(D156:I183, D156) + COUNTIF(D156:I183, F159)</f>
-        <v>111</v>
+        <f>COUNTIF(D156:I189, D156) + COUNTIF(D156:I189, F159)</f>
+        <v>134</v>
       </c>
       <c r="L155" s="18"/>
     </row>
@@ -4030,16 +4200,16 @@
         <v>162</v>
       </c>
       <c r="F159" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G159" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H159" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I159" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J159" s="39"/>
       <c r="K159" s="18"/>
@@ -4124,36 +4294,20 @@
       <c r="L162" s="18"/>
     </row>
     <row r="163" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C163" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="D163" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="E163" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="F163" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="G163" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="H163" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="I163" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="J163" s="45" t="s">
-        <v>193</v>
-      </c>
+      <c r="C163" s="36"/>
+      <c r="D163" s="40"/>
+      <c r="E163" s="40"/>
+      <c r="F163" s="40"/>
+      <c r="G163" s="40"/>
+      <c r="H163" s="40"/>
+      <c r="I163" s="40"/>
+      <c r="J163" s="45"/>
       <c r="K163" s="18"/>
       <c r="L163" s="18"/>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C164" s="41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D164" s="42" t="s">
         <v>162</v>
@@ -4171,13 +4325,13 @@
         <v>162</v>
       </c>
       <c r="I164" s="42" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J164" s="39"/>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C165" s="36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D165" s="40" t="s">
         <v>162</v>
@@ -4202,7 +4356,7 @@
     <row r="166" spans="2:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B166" s="14"/>
       <c r="C166" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D166" s="40" t="s">
         <v>162</v>
@@ -4226,7 +4380,7 @@
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C167" s="36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D167" s="40" t="s">
         <v>162</v>
@@ -4235,7 +4389,7 @@
         <v>162</v>
       </c>
       <c r="F167" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G167" s="40" t="s">
         <v>163</v>
@@ -4250,7 +4404,7 @@
     </row>
     <row r="168" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C168" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D168" s="40" t="s">
         <v>162</v>
@@ -4259,7 +4413,7 @@
         <v>162</v>
       </c>
       <c r="F168" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G168" s="40" t="s">
         <v>163</v>
@@ -4274,7 +4428,7 @@
     </row>
     <row r="169" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C169" s="43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D169" s="44" t="s">
         <v>162</v>
@@ -4297,32 +4451,18 @@
       <c r="J169" s="39"/>
     </row>
     <row r="170" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C170" s="36" t="s">
-        <v>178</v>
-      </c>
-      <c r="D170" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="E170" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="F170" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="G170" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="H170" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="I170" s="40" t="s">
-        <v>163</v>
-      </c>
+      <c r="C170" s="36"/>
+      <c r="D170" s="40"/>
+      <c r="E170" s="40"/>
+      <c r="F170" s="40"/>
+      <c r="G170" s="40"/>
+      <c r="H170" s="40"/>
+      <c r="I170" s="40"/>
       <c r="J170" s="39"/>
     </row>
     <row r="171" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C171" s="41" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D171" s="42" t="s">
         <v>162</v>
@@ -4340,13 +4480,13 @@
         <v>162</v>
       </c>
       <c r="I171" s="42" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J171" s="39"/>
     </row>
     <row r="172" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C172" s="36" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D172" s="40" t="s">
         <v>162</v>
@@ -4370,7 +4510,7 @@
     </row>
     <row r="173" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C173" s="36" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D173" s="40" t="s">
         <v>162</v>
@@ -4385,7 +4525,7 @@
         <v>162</v>
       </c>
       <c r="H173" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I173" s="40" t="s">
         <v>163</v>
@@ -4394,7 +4534,7 @@
     </row>
     <row r="174" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C174" s="36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D174" s="40" t="s">
         <v>162</v>
@@ -4406,7 +4546,7 @@
         <v>162</v>
       </c>
       <c r="G174" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H174" s="40" t="s">
         <v>163</v>
@@ -4418,7 +4558,7 @@
     </row>
     <row r="175" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C175" s="36" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D175" s="40" t="s">
         <v>162</v>
@@ -4430,7 +4570,7 @@
         <v>162</v>
       </c>
       <c r="G175" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H175" s="40" t="s">
         <v>163</v>
@@ -4442,7 +4582,7 @@
     </row>
     <row r="176" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C176" s="43" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D176" s="44" t="s">
         <v>162</v>
@@ -4463,32 +4603,24 @@
         <v>163</v>
       </c>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C177" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="D177" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="E177" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="F177" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="G177" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="H177" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="I177" s="40" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C177" s="36"/>
+      <c r="D177" s="40"/>
+      <c r="E177" s="40"/>
+      <c r="F177" s="40"/>
+      <c r="G177" s="40"/>
+      <c r="H177" s="40"/>
+      <c r="I177" s="40"/>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" s="13">
+        <v>32</v>
+      </c>
+      <c r="B178" s="82" t="s">
+        <v>302</v>
+      </c>
       <c r="C178" s="41" t="s">
-        <v>186</v>
+        <v>298</v>
       </c>
       <c r="D178" s="42" t="s">
         <v>162</v>
@@ -4508,10 +4640,15 @@
       <c r="I178" s="42" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J178" s="39"/>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" s="13">
+        <v>33</v>
+      </c>
+      <c r="B179" s="82"/>
       <c r="C179" s="36" t="s">
-        <v>187</v>
+        <v>303</v>
       </c>
       <c r="D179" s="40" t="s">
         <v>162</v>
@@ -4531,56 +4668,71 @@
       <c r="I179" s="40" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J179" s="39"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="13">
+        <v>34</v>
+      </c>
+      <c r="B180" s="82"/>
       <c r="C180" s="36" t="s">
-        <v>188</v>
+        <v>304</v>
       </c>
       <c r="D180" s="40" t="s">
         <v>162</v>
       </c>
       <c r="E180" s="40" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="F180" s="40" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="G180" s="40" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="H180" s="40" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="I180" s="40" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="J180" s="38"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" s="13">
+        <v>35</v>
+      </c>
+      <c r="B181" s="82"/>
       <c r="C181" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="D181" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E181" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="F181" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="G181" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="D181" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="E181" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="F181" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="G181" s="40" t="s">
-        <v>192</v>
-      </c>
       <c r="H181" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I181" s="40" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="J181" s="38"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" s="13">
+        <v>36</v>
+      </c>
+      <c r="B182" s="82"/>
       <c r="C182" s="36" t="s">
-        <v>190</v>
+        <v>300</v>
       </c>
       <c r="D182" s="40" t="s">
         <v>162</v>
@@ -4592,18 +4744,23 @@
         <v>162</v>
       </c>
       <c r="G182" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H182" s="40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I182" s="40" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="J182" s="38"/>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" s="13">
+        <v>37</v>
+      </c>
+      <c r="B183" s="82"/>
       <c r="C183" s="43" t="s">
-        <v>191</v>
+        <v>301</v>
       </c>
       <c r="D183" s="44" t="s">
         <v>162</v>
@@ -4624,126 +4781,240 @@
         <v>163</v>
       </c>
     </row>
-    <row r="186" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B186" s="11"/>
-      <c r="C186" s="37" t="s">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C184" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="D184" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E184" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="F184" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="G184" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="H184" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="I184" s="42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C185" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="D185" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E185" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="F185" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="G185" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="H185" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="I185" s="40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C186" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="D186" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E186" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="F186" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="G186" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="H186" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="I186" s="40" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C187" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D187" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E187" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="F187" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="G187" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="H187" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="I187" s="40" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C188" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="D188" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E188" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="F188" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="G188" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="H188" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="I188" s="40" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C189" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="D189" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="E189" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="F189" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="G189" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="H189" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="I189" s="44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B192" s="11"/>
+      <c r="C192" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D192" s="37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C193" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="D193" s="38" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C194" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="D186" s="37" t="s">
+      <c r="D194" s="38" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="187" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C187" s="36" t="s">
+    <row r="195" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C195" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="D187" s="38" t="s">
+      <c r="D195" s="38" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="188" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C188" s="36" t="s">
+    <row r="196" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C196" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="D188" s="38" t="s">
+      <c r="D196" s="38" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="189" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C189" s="36" t="s">
+    <row r="199" spans="2:4" ht="92.25" x14ac:dyDescent="0.4">
+      <c r="B199" s="11">
+        <v>45852</v>
+      </c>
+      <c r="C199" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="D189" s="38" t="s">
+    </row>
+    <row r="200" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C200" s="46" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="190" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C190" s="36" t="s">
+      <c r="D200" s="46"/>
+    </row>
+    <row r="202" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C202" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="D190" s="38" t="s">
+    </row>
+    <row r="203" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C203" s="46" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="193" spans="2:4" ht="92.25" x14ac:dyDescent="0.4">
-      <c r="B193" s="11">
-        <v>45852</v>
-      </c>
-      <c r="C193" s="46" t="s">
+    <row r="204" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C204" s="46" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="194" spans="2:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="C194" s="46" t="s">
+    <row r="205" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C205" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="D194" s="46"/>
-    </row>
-    <row r="196" spans="2:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="C196" s="46" t="s">
+    </row>
+    <row r="206" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C206" s="46" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="197" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C197" s="46" t="s">
+    <row r="207" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C207" s="46" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="198" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="C198" s="46" t="s">
+    <row r="208" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C208" s="46" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="199" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C199" s="46" t="s">
+    <row r="210" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B210" s="11">
+        <v>45853</v>
+      </c>
+      <c r="C210" s="47" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="200" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C200" s="46" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="201" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C201" s="46" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="202" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C202" s="46" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="204" spans="2:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B204" s="11">
-        <v>45853</v>
-      </c>
-      <c r="C204" s="47" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C205" s="48"/>
-    </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C206" s="49" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C207" s="48"/>
-    </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C208" s="49" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C209" s="48"/>
-    </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C210" s="49" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="211" spans="2:7" x14ac:dyDescent="0.25">
@@ -4751,7 +5022,7 @@
     </row>
     <row r="212" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C212" s="49" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
@@ -4759,103 +5030,94 @@
     </row>
     <row r="214" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C214" s="49" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="215" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C215" s="48"/>
+    </row>
+    <row r="216" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C216" s="49" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="217" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C217" s="48"/>
+    </row>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C218" s="49" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="219" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C219" s="48"/>
+    </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C220" s="49" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="223" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B223" s="11">
+        <v>45857</v>
+      </c>
+      <c r="C223" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="D223" s="37" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="217" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B217" s="11">
-        <v>45857</v>
-      </c>
-      <c r="C217" s="50" t="s">
-        <v>228</v>
-      </c>
-      <c r="D217" s="37" t="s">
+      <c r="E223" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="G223" s="51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="224" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C224" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="D224" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="E224" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="G224"/>
+    </row>
+    <row r="225" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C225" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="D225" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="E225" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="G225" s="52" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="226" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C226" s="38"/>
+      <c r="D226" s="38"/>
+      <c r="E226" s="38"/>
+      <c r="G226" s="48"/>
+    </row>
+    <row r="227" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C227" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="E217" s="37" t="s">
+      <c r="D227" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="G217" s="51" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C218" s="38" t="s">
-        <v>224</v>
-      </c>
-      <c r="D218" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="E218" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="G218"/>
-    </row>
-    <row r="219" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C219" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="D219" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="E219" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="G219" s="52" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C220" s="38"/>
-      <c r="D220" s="38"/>
-      <c r="E220" s="38"/>
-      <c r="G220" s="48"/>
-    </row>
-    <row r="221" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C221" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="D221" s="38" t="s">
+      <c r="E227" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="G227" s="48" t="s">
         <v>227</v>
-      </c>
-      <c r="E221" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="G221" s="48" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="222" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G222" s="48"/>
-    </row>
-    <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G223" s="48" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="224" spans="2:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="C224" s="53" t="s">
-        <v>239</v>
-      </c>
-      <c r="G224" s="48"/>
-    </row>
-    <row r="225" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C225" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="G225" s="48" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="226" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C226" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="G226"/>
-    </row>
-    <row r="227" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G227" s="52" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="228" spans="3:7" x14ac:dyDescent="0.25">
@@ -4863,75 +5125,251 @@
     </row>
     <row r="229" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G229" s="48" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="3:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="C230" s="53" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="230" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G230" s="48"/>
     </row>
     <row r="231" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C231" s="13" t="s">
+        <v>234</v>
+      </c>
       <c r="G231" s="48" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="232" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G232" s="48"/>
-    </row>
-    <row r="233" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G233" s="48" t="s">
+      <c r="C232" s="13" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="244" spans="3:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="C244" s="51" t="s">
+      <c r="G232"/>
+    </row>
+    <row r="233" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G233" s="52" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="234" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G234" s="48"/>
+    </row>
+    <row r="235" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G235" s="48" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="236" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G236" s="48"/>
+    </row>
+    <row r="237" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G237" s="48" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="238" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G238" s="48"/>
+    </row>
+    <row r="239" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G239" s="48" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="250" spans="3:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="C250" s="51" t="s">
+        <v>239</v>
+      </c>
+      <c r="E250" s="51" t="s">
         <v>243</v>
       </c>
-      <c r="E244" s="51" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="245" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C245" s="48"/>
-      <c r="E245" s="48"/>
-    </row>
-    <row r="246" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C246" s="48" t="s">
+    </row>
+    <row r="251" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C251" s="48"/>
+      <c r="E251" s="48"/>
+    </row>
+    <row r="252" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C252" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="E252" s="48" t="s">
         <v>244</v>
       </c>
-      <c r="E246" s="48" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="247" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C247" s="48"/>
-      <c r="E247" s="48"/>
-    </row>
-    <row r="248" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C248" s="48" t="s">
+    </row>
+    <row r="253" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C253" s="48"/>
+      <c r="E253" s="48"/>
+    </row>
+    <row r="254" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C254" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="E254" s="48" t="s">
         <v>245</v>
       </c>
-      <c r="E248" s="48" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="249" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C249" s="48"/>
-      <c r="E249" s="48"/>
-    </row>
-    <row r="250" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C250" s="48" t="s">
+    </row>
+    <row r="255" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C255" s="48"/>
+      <c r="E255" s="48"/>
+    </row>
+    <row r="256" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C256" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="E256" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="E250" s="48" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C292" s="13" t="s">
+    </row>
+    <row r="298" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C298" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="300" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B300" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="C300" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D300" s="13" t="s">
         <v>261</v>
       </c>
+      <c r="E300" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="301" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B301" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C301" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D301" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="E301" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="302" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B302" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C302" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D302" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="E302" s="13" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="303" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B303" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C303" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D303" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="E303" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="304" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B304" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C304" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="D304" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="E304" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="305" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B305" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C305" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D305" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="E305" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="306" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B306" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="C306" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="D306" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="E306" s="13" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="307" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B307" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="C307" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="D307" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="E307" s="13" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="308" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B308" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="C308" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="D308" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E308" s="13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="309" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B309" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C309" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="D309" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="E309" s="13" t="s">
+        <v>297</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B178:B183"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
GĐ 7-2: Hoàn thiện giao diện và logic xử lý file; cập nhật các view liên quan, đồng thời điều chỉnh controller và model của Task và Comment để tích hợp chức năng này.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECF1F1C-E766-4C4D-B4E1-541FDA632541}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D888934C-638B-4C9F-8AD5-F97CDD9B5F55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -1901,6 +1901,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1928,64 +1985,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2081,7 +2081,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>537745</xdr:colOff>
+      <xdr:colOff>469709</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>73244</xdr:rowOff>
     </xdr:to>
@@ -2125,7 +2125,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>110042</xdr:colOff>
+      <xdr:colOff>42006</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>111301</xdr:rowOff>
     </xdr:to>
@@ -2213,7 +2213,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>644002</xdr:colOff>
+      <xdr:colOff>575967</xdr:colOff>
       <xdr:row>147</xdr:row>
       <xdr:rowOff>34709</xdr:rowOff>
     </xdr:to>
@@ -2345,7 +2345,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1643006</xdr:colOff>
+      <xdr:colOff>1574971</xdr:colOff>
       <xdr:row>272</xdr:row>
       <xdr:rowOff>112351</xdr:rowOff>
     </xdr:to>
@@ -2433,7 +2433,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>378479</xdr:colOff>
+      <xdr:colOff>310444</xdr:colOff>
       <xdr:row>292</xdr:row>
       <xdr:rowOff>33922</xdr:rowOff>
     </xdr:to>
@@ -2758,7 +2758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:C12"/>
     </sheetView>
   </sheetViews>
@@ -2778,31 +2778,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="67"/>
+      <c r="E3" s="61"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="67"/>
+      <c r="E4" s="61"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2810,12 +2810,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="68" t="s">
+      <c r="H5" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2853,19 +2853,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="70">
+      <c r="A7" s="64">
         <v>1</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="73" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="67" t="s">
         <v>251</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="70" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="21"/>
@@ -2882,11 +2882,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="77"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="71"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2903,11 +2903,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="77"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="71"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -2924,11 +2924,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="77"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="71"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -2943,11 +2943,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="77"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="71"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -2964,11 +2964,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="78"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="72"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -2983,19 +2983,19 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="57">
+      <c r="A13" s="76">
         <v>2</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="57" t="s">
+      <c r="D13" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="82" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="21"/>
@@ -3012,11 +3012,11 @@
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="64"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="83"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
@@ -3029,11 +3029,11 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="65"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="84"/>
       <c r="H15" s="27" t="s">
         <v>247</v>
       </c>
@@ -3141,10 +3141,10 @@
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
       <c r="E20" s="7"/>
-      <c r="H20" s="83"/>
+      <c r="H20" s="57"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="84"/>
-      <c r="K20" s="85"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
     </row>
     <row r="21" spans="1:11" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -3172,6 +3172,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -3181,11 +3186,6 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1048576 E1:E14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3204,8 +3204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
   <dimension ref="A4:P309"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M172" sqref="M172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3216,7 +3216,9 @@
     <col min="4" max="4" width="78.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="13" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="13" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="13"/>
     <col min="11" max="11" width="25.5703125" style="13" customWidth="1"/>
     <col min="12" max="14" width="9.140625" style="13"/>
@@ -4107,7 +4109,7 @@
       <c r="J155" s="33"/>
       <c r="K155">
         <f>COUNTIF(D156:I189, D156) + COUNTIF(D156:I189, F159)</f>
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L155" s="18"/>
     </row>
@@ -4522,7 +4524,7 @@
         <v>162</v>
       </c>
       <c r="G173" s="40" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="H173" s="40" t="s">
         <v>189</v>
@@ -4616,7 +4618,7 @@
       <c r="A178" s="13">
         <v>32</v>
       </c>
-      <c r="B178" s="82" t="s">
+      <c r="B178" s="85" t="s">
         <v>302</v>
       </c>
       <c r="C178" s="41" t="s">
@@ -4646,7 +4648,7 @@
       <c r="A179" s="13">
         <v>33</v>
       </c>
-      <c r="B179" s="82"/>
+      <c r="B179" s="85"/>
       <c r="C179" s="36" t="s">
         <v>303</v>
       </c>
@@ -4666,7 +4668,7 @@
         <v>162</v>
       </c>
       <c r="I179" s="40" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J179" s="39"/>
     </row>
@@ -4674,7 +4676,7 @@
       <c r="A180" s="13">
         <v>34</v>
       </c>
-      <c r="B180" s="82"/>
+      <c r="B180" s="85"/>
       <c r="C180" s="36" t="s">
         <v>304</v>
       </c>
@@ -4702,7 +4704,7 @@
       <c r="A181" s="13">
         <v>35</v>
       </c>
-      <c r="B181" s="82"/>
+      <c r="B181" s="85"/>
       <c r="C181" s="36" t="s">
         <v>299</v>
       </c>
@@ -4722,7 +4724,7 @@
         <v>189</v>
       </c>
       <c r="I181" s="40" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="J181" s="38"/>
     </row>
@@ -4730,7 +4732,7 @@
       <c r="A182" s="13">
         <v>36</v>
       </c>
-      <c r="B182" s="82"/>
+      <c r="B182" s="85"/>
       <c r="C182" s="36" t="s">
         <v>300</v>
       </c>
@@ -4750,7 +4752,7 @@
         <v>189</v>
       </c>
       <c r="I182" s="40" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="J182" s="38"/>
     </row>
@@ -4758,7 +4760,7 @@
       <c r="A183" s="13">
         <v>37</v>
       </c>
-      <c r="B183" s="82"/>
+      <c r="B183" s="85"/>
       <c r="C183" s="43" t="s">
         <v>301</v>
       </c>

</xml_diff>

<commit_message>
GĐ 8-1: Tiến hành xoá các file không sử dụng, refactor lại code trong CommentController, CommentService và CommentPolicy. Đồng thời cập nhật các file liên quan.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D888934C-638B-4C9F-8AD5-F97CDD9B5F55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2F6830-93D8-4E7E-BC49-677D2B03B96E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
-    <sheet name="Note work" sheetId="2" r:id="rId2"/>
+    <sheet name="Role - Permission" sheetId="3" r:id="rId2"/>
+    <sheet name="Note work" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="307">
   <si>
     <t>STT</t>
   </si>
@@ -1480,12 +1481,15 @@
   <si>
     <t>File</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1616,6 +1620,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1637,7 +1647,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1755,11 +1765,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1908,6 +1963,31 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2758,7 +2838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:C12"/>
     </sheetView>
   </sheetViews>
@@ -2778,31 +2858,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="61"/>
+      <c r="E3" s="70"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="61"/>
+      <c r="E4" s="70"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2810,12 +2890,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2853,19 +2933,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="64">
+      <c r="A7" s="73">
         <v>1</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="82" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="76" t="s">
         <v>251</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="79" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="21"/>
@@ -2882,11 +2962,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="65"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="71"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2903,11 +2983,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="71"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="80"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -2924,11 +3004,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="71"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="80"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -2943,11 +3023,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="71"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="80"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -2964,11 +3044,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="72"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="81"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -2983,19 +3063,19 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="76">
+      <c r="A13" s="85">
         <v>2</v>
       </c>
-      <c r="B13" s="76" t="s">
+      <c r="B13" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="76" t="s">
+      <c r="D13" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="82" t="s">
+      <c r="E13" s="91" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="21"/>
@@ -3012,11 +3092,11 @@
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="83"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="92"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
@@ -3029,11 +3109,11 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="78"/>
-      <c r="B15" s="78"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="84"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="93"/>
       <c r="H15" s="27" t="s">
         <v>247</v>
       </c>
@@ -3201,11 +3281,826 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1202BCE7-7D77-44EA-8C50-935D6D7AD06E}">
+  <dimension ref="C4:L40"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="8"/>
+    <col min="3" max="3" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="K4" s="60" t="s">
+        <v>306</v>
+      </c>
+      <c r="L4" s="60">
+        <f>COUNTIF($D$5:$I$40, D5) + COUNTIF($D$5:$I$40, F9)</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" s="62" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="63"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H7" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F9" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="G9" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H9" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="I9" s="64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F10" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H10" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I11" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="63" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F12" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G12" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H14" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I14" s="64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G15" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I15" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F16" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G16" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H16" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I16" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F17" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="G17" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H17" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I17" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F18" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="G18" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H18" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I18" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G19" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I19" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="63"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="63" t="s">
+        <v>177</v>
+      </c>
+      <c r="D21" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F21" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H21" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I21" s="64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="63" t="s">
+        <v>178</v>
+      </c>
+      <c r="D22" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F22" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H22" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I22" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="63" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H23" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="I23" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F24" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G24" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H24" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I24" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G25" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H25" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I25" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="63" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F26" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H26" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I26" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="63"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="63" t="s">
+        <v>298</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F28" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G28" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H28" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I28" s="64" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="63" t="s">
+        <v>303</v>
+      </c>
+      <c r="D29" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F29" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H29" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I29" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="63" t="s">
+        <v>304</v>
+      </c>
+      <c r="D30" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E30" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F30" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H30" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I30" s="64" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="63" t="s">
+        <v>299</v>
+      </c>
+      <c r="D31" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E31" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F31" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G31" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H31" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="I31" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="63" t="s">
+        <v>300</v>
+      </c>
+      <c r="D32" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E32" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F32" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G32" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H32" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="I32" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="63" t="s">
+        <v>301</v>
+      </c>
+      <c r="D33" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G33" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H33" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I33" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="63"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D35" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E35" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F35" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I35" s="64" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="D36" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F36" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H36" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="64" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="63" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="F37" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="G37" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H37" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="I37" s="64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="D38" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F38" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G38" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H38" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="I38" s="64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="D39" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E39" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F39" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H39" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="I39" s="64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="D40" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E40" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="F40" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="G40" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="H40" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="I40" s="68" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2427CB-E0F8-4CD5-B6B8-B17AA84BAAA6}">
   <dimension ref="A4:P309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M172" sqref="M172"/>
+    <sheetView topLeftCell="A150" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K155" sqref="K155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4618,7 +5513,7 @@
       <c r="A178" s="13">
         <v>32</v>
       </c>
-      <c r="B178" s="85" t="s">
+      <c r="B178" s="94" t="s">
         <v>302</v>
       </c>
       <c r="C178" s="41" t="s">
@@ -4648,7 +5543,7 @@
       <c r="A179" s="13">
         <v>33</v>
       </c>
-      <c r="B179" s="85"/>
+      <c r="B179" s="94"/>
       <c r="C179" s="36" t="s">
         <v>303</v>
       </c>
@@ -4676,7 +5571,7 @@
       <c r="A180" s="13">
         <v>34</v>
       </c>
-      <c r="B180" s="85"/>
+      <c r="B180" s="94"/>
       <c r="C180" s="36" t="s">
         <v>304</v>
       </c>
@@ -4704,7 +5599,7 @@
       <c r="A181" s="13">
         <v>35</v>
       </c>
-      <c r="B181" s="85"/>
+      <c r="B181" s="94"/>
       <c r="C181" s="36" t="s">
         <v>299</v>
       </c>
@@ -4732,7 +5627,7 @@
       <c r="A182" s="13">
         <v>36</v>
       </c>
-      <c r="B182" s="85"/>
+      <c r="B182" s="94"/>
       <c r="C182" s="36" t="s">
         <v>300</v>
       </c>
@@ -4760,7 +5655,7 @@
       <c r="A183" s="13">
         <v>37</v>
       </c>
-      <c r="B183" s="85"/>
+      <c r="B183" s="94"/>
       <c r="C183" s="43" t="s">
         <v>301</v>
       </c>

</xml_diff>

<commit_message>
GĐ 8-2: Refactor lại code trong FileController, FileService, FilePolicy; cập nhật các view liên quan.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2F6830-93D8-4E7E-BC49-677D2B03B96E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4726B53-34E2-41CB-8463-4B4724558F25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1990,6 +1990,33 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2037,33 +2064,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2858,31 +2858,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="70"/>
+      <c r="E3" s="79"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="70"/>
+      <c r="E4" s="79"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2890,12 +2890,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="71" t="s">
+      <c r="H5" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2933,19 +2933,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="73">
+      <c r="A7" s="82">
         <v>1</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="91" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="85" t="s">
         <v>251</v>
       </c>
-      <c r="E7" s="79" t="s">
+      <c r="E7" s="88" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="21"/>
@@ -2962,11 +2962,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="74"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="80"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="89"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2983,11 +2983,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="80"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="89"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -3004,11 +3004,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="74"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="80"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="89"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -3023,11 +3023,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="80"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="89"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -3044,11 +3044,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="81"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="90"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -3063,19 +3063,19 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="85">
+      <c r="A13" s="69">
         <v>2</v>
       </c>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="85" t="s">
+      <c r="D13" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="91" t="s">
+      <c r="E13" s="75" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="21"/>
@@ -3092,11 +3092,11 @@
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="92"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="76"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
@@ -3109,11 +3109,11 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="87"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="93"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="77"/>
       <c r="H15" s="27" t="s">
         <v>247</v>
       </c>
@@ -3252,11 +3252,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -3266,6 +3261,11 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1048576 E1:E14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3284,8 +3284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1202BCE7-7D77-44EA-8C50-935D6D7AD06E}">
   <dimension ref="C4:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
GĐ 8-4: Refactor lại code trong ProjectController, ProjectService và ProjectPolicy, tập trung phần phân quyền. Đồng thời cập nhật các file liên quan để đồng bộ logic phân quyền. Điều chỉnh lệnh hiển thị phân trang data->links() thành data?->links() để tránh lỗi khi không có dữ liệu.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4726B53-34E2-41CB-8463-4B4724558F25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FDF74D-554C-4F02-B20C-4B8F9F40B6FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1990,6 +1990,54 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2016,54 +2064,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2858,31 +2858,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="79"/>
+      <c r="E3" s="70"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="79"/>
+      <c r="E4" s="70"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2890,12 +2890,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="80" t="s">
+      <c r="H5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2933,19 +2933,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="82">
+      <c r="A7" s="73">
         <v>1</v>
       </c>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="91" t="s">
+      <c r="C7" s="82" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="85" t="s">
+      <c r="D7" s="76" t="s">
         <v>251</v>
       </c>
-      <c r="E7" s="88" t="s">
+      <c r="E7" s="79" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="21"/>
@@ -2962,11 +2962,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="83"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="89"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="80"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2983,11 +2983,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="89"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="80"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -3004,11 +3004,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="89"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="80"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -3023,11 +3023,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="89"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="80"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -3044,11 +3044,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="84"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="90"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="81"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -3063,19 +3063,19 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="69">
+      <c r="A13" s="85">
         <v>2</v>
       </c>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="69" t="s">
+      <c r="D13" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="91" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="21"/>
@@ -3092,11 +3092,11 @@
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="70"/>
-      <c r="B14" s="70"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="76"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="92"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
@@ -3109,11 +3109,11 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="77"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="93"/>
       <c r="H15" s="27" t="s">
         <v>247</v>
       </c>
@@ -3252,6 +3252,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -3261,11 +3266,6 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1048576 E1:E14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3284,8 +3284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1202BCE7-7D77-44EA-8C50-935D6D7AD06E}">
   <dimension ref="C4:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3567,7 +3567,7 @@
         <v>162</v>
       </c>
       <c r="F16" s="64" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="G16" s="67" t="s">
         <v>163</v>
@@ -3841,10 +3841,10 @@
         <v>162</v>
       </c>
       <c r="G29" s="64" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="H29" s="64" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="I29" s="67" t="s">
         <v>163</v>

</xml_diff>

<commit_message>
GĐ 8-5: Refactor lại code trong UserController, UserService, UserPolicy, tập trung phần phân quyền; Đồng thời cập nhật các file liên quan; Thêm quyền reset-password.
</commit_message>
<xml_diff>
--- a/Schedule-Note.xlsx
+++ b/Schedule-Note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\task-manager-laravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FDF74D-554C-4F02-B20C-4B8F9F40B6FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2289DB6-E608-4F3C-A732-D6B32AFAB84A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="308">
   <si>
     <t>STT</t>
   </si>
@@ -1483,6 +1483,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>user.reset-password</t>
   </si>
 </sst>
 </file>
@@ -1990,6 +1993,33 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2037,33 +2067,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2858,31 +2861,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="70"/>
+      <c r="E3" s="79"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="70"/>
+      <c r="E4" s="79"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -2890,12 +2893,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="H5" s="71" t="s">
+      <c r="H5" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2933,19 +2936,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="73">
+      <c r="A7" s="82">
         <v>1</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="91" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="85" t="s">
         <v>251</v>
       </c>
-      <c r="E7" s="79" t="s">
+      <c r="E7" s="88" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="21"/>
@@ -2962,11 +2965,11 @@
       <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="74"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="80"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="89"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="24" t="s">
@@ -2983,11 +2986,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="80"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="89"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="24" t="s">
@@ -3004,11 +3007,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="74"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="80"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="89"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="24" t="s">
@@ -3023,11 +3026,11 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="80"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="89"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="24" t="s">
@@ -3044,11 +3047,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="81"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="90"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="24" t="s">
@@ -3063,19 +3066,19 @@
       <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="85">
+      <c r="A13" s="69">
         <v>2</v>
       </c>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="85" t="s">
+      <c r="D13" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="91" t="s">
+      <c r="E13" s="75" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="21"/>
@@ -3092,11 +3095,11 @@
       <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="92"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="76"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="27" t="s">
@@ -3109,11 +3112,11 @@
       <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="87"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="93"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="77"/>
       <c r="H15" s="27" t="s">
         <v>247</v>
       </c>
@@ -3252,11 +3255,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -3266,6 +3264,11 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="D7:D12"/>
     <mergeCell ref="C7:C12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1048576 E1:E14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -3282,16 +3285,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1202BCE7-7D77-44EA-8C50-935D6D7AD06E}">
-  <dimension ref="C4:L40"/>
+  <dimension ref="C4:L41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="8"/>
-    <col min="3" max="3" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
@@ -3327,8 +3330,8 @@
         <v>306</v>
       </c>
       <c r="L4" s="60">
-        <f>COUNTIF($D$5:$I$40, D5) + COUNTIF($D$5:$I$40, F9)</f>
-        <v>131</v>
+        <f>COUNTIF($D$5:$I$41, D5) + COUNTIF($D$5:$I$41, F9)</f>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="3:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3502,40 +3505,40 @@
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C13" s="63"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
+      <c r="C13" s="63" t="s">
+        <v>307</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G13" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H13" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13" s="67" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C14" s="63" t="s">
-        <v>171</v>
-      </c>
-      <c r="D14" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="F14" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="G14" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="H14" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="I14" s="64" t="s">
-        <v>189</v>
-      </c>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15" s="64" t="s">
         <v>162</v>
@@ -3546,19 +3549,19 @@
       <c r="F15" s="64" t="s">
         <v>162</v>
       </c>
-      <c r="G15" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="H15" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="I15" s="67" t="s">
-        <v>163</v>
+      <c r="G15" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H15" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I15" s="64" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D16" s="64" t="s">
         <v>162</v>
@@ -3567,7 +3570,7 @@
         <v>162</v>
       </c>
       <c r="F16" s="64" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="G16" s="67" t="s">
         <v>163</v>
@@ -3581,7 +3584,7 @@
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D17" s="64" t="s">
         <v>162</v>
@@ -3604,7 +3607,7 @@
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D18" s="64" t="s">
         <v>162</v>
@@ -3627,62 +3630,62 @@
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="G19" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I19" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="D19" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="E19" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="F19" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="G19" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="H19" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="I19" s="67" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="63"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
+      <c r="D20" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F20" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G20" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H20" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I20" s="67" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="D21" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="E21" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="F21" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="G21" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="H21" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="I21" s="64" t="s">
-        <v>189</v>
-      </c>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D22" s="64" t="s">
         <v>162</v>
@@ -3696,16 +3699,16 @@
       <c r="G22" s="64" t="s">
         <v>162</v>
       </c>
-      <c r="H22" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="I22" s="67" t="s">
-        <v>163</v>
+      <c r="H22" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="I22" s="64" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D23" s="64" t="s">
         <v>162</v>
@@ -3717,10 +3720,10 @@
         <v>162</v>
       </c>
       <c r="G23" s="64" t="s">
-        <v>189</v>
-      </c>
-      <c r="H23" s="64" t="s">
-        <v>189</v>
+        <v>162</v>
+      </c>
+      <c r="H23" s="67" t="s">
+        <v>163</v>
       </c>
       <c r="I23" s="67" t="s">
         <v>163</v>
@@ -3728,7 +3731,7 @@
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D24" s="64" t="s">
         <v>162</v>
@@ -3742,8 +3745,8 @@
       <c r="G24" s="64" t="s">
         <v>189</v>
       </c>
-      <c r="H24" s="67" t="s">
-        <v>163</v>
+      <c r="H24" s="64" t="s">
+        <v>189</v>
       </c>
       <c r="I24" s="67" t="s">
         <v>163</v>
@@ -3751,7 +3754,7 @@
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="63" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D25" s="64" t="s">
         <v>162</v>
@@ -3774,62 +3777,62 @@
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="D26" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F26" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G26" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H26" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I26" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="D26" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="E26" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="F26" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="G26" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="H26" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="I26" s="67" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="63"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
+      <c r="D27" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F27" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G27" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H27" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I27" s="67" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="63" t="s">
-        <v>298</v>
-      </c>
-      <c r="D28" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="E28" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="F28" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="G28" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="H28" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="I28" s="64" t="s">
-        <v>162</v>
-      </c>
+      <c r="C28" s="63"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="64"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="63" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D29" s="64" t="s">
         <v>162</v>
@@ -3841,18 +3844,18 @@
         <v>162</v>
       </c>
       <c r="G29" s="64" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="H29" s="64" t="s">
-        <v>189</v>
-      </c>
-      <c r="I29" s="67" t="s">
-        <v>163</v>
+        <v>162</v>
+      </c>
+      <c r="I29" s="64" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" s="63" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D30" s="64" t="s">
         <v>162</v>
@@ -3864,18 +3867,18 @@
         <v>162</v>
       </c>
       <c r="G30" s="64" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="H30" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="I30" s="64" t="s">
-        <v>162</v>
+        <v>189</v>
+      </c>
+      <c r="I30" s="67" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="63" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="D31" s="64" t="s">
         <v>162</v>
@@ -3887,18 +3890,18 @@
         <v>162</v>
       </c>
       <c r="G31" s="64" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="H31" s="64" t="s">
-        <v>189</v>
-      </c>
-      <c r="I31" s="67" t="s">
-        <v>163</v>
+        <v>162</v>
+      </c>
+      <c r="I31" s="64" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="63" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D32" s="64" t="s">
         <v>162</v>
@@ -3921,62 +3924,62 @@
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="63" t="s">
+        <v>300</v>
+      </c>
+      <c r="D33" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G33" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H33" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="I33" s="67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="63" t="s">
         <v>301</v>
       </c>
-      <c r="D33" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="E33" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="F33" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="G33" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="H33" s="67" t="s">
-        <v>163</v>
-      </c>
-      <c r="I33" s="67" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="63"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
+      <c r="D34" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F34" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="H34" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I34" s="67" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C35" s="63" t="s">
-        <v>183</v>
-      </c>
-      <c r="D35" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="E35" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="F35" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="G35" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="H35" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="I35" s="64" t="s">
-        <v>162</v>
-      </c>
+      <c r="C35" s="63"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="63" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D36" s="64" t="s">
         <v>162</v>
@@ -3999,39 +4002,39 @@
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D37" s="64" t="s">
         <v>162</v>
       </c>
       <c r="E37" s="64" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="F37" s="64" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="G37" s="64" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="H37" s="64" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="I37" s="64" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D38" s="64" t="s">
         <v>162</v>
       </c>
       <c r="E38" s="64" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="F38" s="64" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
       <c r="G38" s="64" t="s">
         <v>189</v>
@@ -4045,7 +4048,7 @@
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D39" s="64" t="s">
         <v>162</v>
@@ -4067,25 +4070,48 @@
       </c>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="65" t="s">
+      <c r="C40" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="E40" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="F40" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G40" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="H40" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="I40" s="64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="D40" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="E40" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="F40" s="68" t="s">
-        <v>163</v>
-      </c>
-      <c r="G40" s="68" t="s">
-        <v>163</v>
-      </c>
-      <c r="H40" s="68" t="s">
-        <v>163</v>
-      </c>
-      <c r="I40" s="68" t="s">
+      <c r="D41" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="E41" s="66" t="s">
+        <v>162</v>
+      </c>
+      <c r="F41" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="G41" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="H41" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="I41" s="68" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>